<commit_message>
Atualizado iframe001 e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97993882-D867-4A05-8953-C4DDCF7D866D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8AF34-6D9A-4A2B-B6D6-90A032BDE687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,19 +25,921 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
   <si>
     <t>flexbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capítulo 22 </t>
+  </si>
+  <si>
+    <t>Aula 01 - Nosso primeiro iframe</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"http://cursoemvideo.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>frameborder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"http://thiagocamponez.github.io/projeto"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>frameborder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Obs.:</t>
+  </si>
+  <si>
+    <t>No src coloca o site que deseja abrir no iframe</t>
+  </si>
+  <si>
+    <t>frameborder é a largura da borda</t>
+  </si>
+  <si>
+    <t>Não é todo site que deixa ser exibido em um iframe</t>
+  </si>
+  <si>
+    <t>Aula 2 – Configurações do iframe</t>
+  </si>
+  <si>
+    <t>Nem todo navegador de site é compatível para abrir o iframe, então dentro da tag iframe coloque a tag &lt;a&gt; com o link do site.</t>
+  </si>
+  <si>
+    <t>TAMANHO PADRÃO de um iframe é 300x150 mas é possível definir outro tamanho com css</t>
+  </si>
+  <si>
+    <t>O scolling serve para tirar a rolagem do iframe, mas somente no macbook da aple, nos google chrome do windows não tira...</t>
+  </si>
+  <si>
+    <t>O frameborder só tem 2 tipos, o 0 e 1 (qualquer outro número ficará com a config do 1) podendo colocar borda no css</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Estudos de iframe&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>height</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>head</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Testando o uso de um iframe&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt;Acessando o site do </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"https://cursoemvideo.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>frameborder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>height</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"500"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>scolling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"no"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"https://www.cursoemvideo.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Curso em Vídeo&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        para aprender programar.&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Aula 3 – Conteúdo local no iframe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +947,94 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE1E1E6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF988BC7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE7DE79"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF79C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF78D1E1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF67E480"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -62,12 +1042,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,26 +1444,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="153.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="8"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="8"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="8"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="8"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="8"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="8"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="8"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="8"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="8"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="8"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="8"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" s="8"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="8"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="8"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" s="8"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="8"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="8"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="8"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="8"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="8"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="8"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="8"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="8"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="8"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="7"/>
+      <c r="B80" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A80"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criei o iframe002, pg001 e atualizei a planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8AF34-6D9A-4A2B-B6D6-90A032BDE687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6FA11-331E-4D96-98DC-7634884D2566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -933,6 +933,353 @@
   </si>
   <si>
     <t>Aula 3 – Conteúdo local no iframe</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Teste com iframe&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"pg001.html"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>frameborder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>height</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"500"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"500"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Lorem ipsum, dolor sit amet consectetur adipisicing elit. Officiis eum dolore facere aliquam. 
+Quae adipisci blanditiis quas perspiciatis, ducimus quo, minus expedita quam sed quos alias odio earum id fugiat. 
+Lorem ipsum dolor sit amet consectetur adipisicing elit. Mollitia vero temporibus enim totam, culpa, 
+quisquam quia beatae saepe corporis facilis soluta explicabo, aspernatur sequi. In esse labore natus quod a.&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Lorem ipsum, dolor sit amet consectetur adipisicing elit. Reiciendis, illo minus asperiores repudiandae et maxime. 
+Voluptatibus fuga magnam ipsa? Beatae aliquid commodi vero quae expedita repellat dolores porro, ut assumenda? 
+Lorem ipsum, dolor sit amet consectetur adipisicing elit. Earum illum cupiditate dolores unde temporibus doloribus fugit iure, 
+sed maxime quo soluta tempore voluptatem! Sunt necessitatibus dolorum vero omnis tenetur corrupti?&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Ensina que é possível colocar uma página própria em um iframe, deu o exemplo de colocar a última tabela feita no módulo 3</t>
+  </si>
+  <si>
+    <t>Mas disse que se for usar tabela é melhor utilizar da outra forma mesmo - usando a div container</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1110,15 +1457,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1129,6 +1467,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1446,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
   <dimension ref="A2:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,368 +1817,386 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="9"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="11" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="8" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="9" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="8"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="8"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="9"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="8"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="9"/>
+    </row>
+    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="8"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="8"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="8"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="8"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="8"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="8"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="8"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="8"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="8"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="8"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="8"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="8"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="8"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="8"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="8"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="8"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="8"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="8"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="8"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="8"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="8"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="8"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="8"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="8"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="8"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="7"/>
-      <c r="B80" s="10"/>
+      <c r="A80" s="12"/>
+      <c r="B80" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Alterado o iframe002, criado o iframe003, pag001, pag002 e pag003 e alterada a planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6FA11-331E-4D96-98DC-7634884D2566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E59F2D-62D2-427B-B91C-1D30C505AEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -1280,6 +1280,798 @@
   </si>
   <si>
     <t>Mas disse que se for usar tabela é melhor utilizar da outra forma mesmo - usando a div container</t>
+  </si>
+  <si>
+    <t>Aula 4 – Navegação no iframe</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Faça uma escolha&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ul</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"paginas-extras/pag001.html"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"frame"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Primeira Lista&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"paginas-extras/pag002.html"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"frame"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Segunda Lista&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;            </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"paginas-extras/pag003.html"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"frame"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Terceira Lista&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ul</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tela"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"frame"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Infelizmente o seu navegador não é compatível com isso.&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Lorem ipsum dolor sit amet consectetur adipisicing elit. Ex odio ipsum inventore officiis laboriosam pariatur laborum 
+cupiditate porro doloremque, nesciunt incidunt quo, perferendis autem praesentium sapiente soluta, quas non! Nostrum.&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Lorem ipsum, dolor sit amet consectetur adipisicing elit. Quod quae quisquam, dolores libero ratione distinctio
+ perspiciatis, numquam sit tenetur atque dolor similique, sapiente ducimus omnis reiciendis non! Quisquam, nobis natus? Lorem ipsum dolor sit amet consectetur adipisicing elit. Ab sapiente animi possimus tempore atque? Consectetur consequuntur accusamus, velit ea quaerat est vero ex quibusdam voluptatibus minus. Vitae, eum doloremque! Ea!&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Lorem ipsum dolor sit amet, consectetur adipisicing elit. Voluptate laudantium voluptatibus, beatae atque quam dolores 
+tenetur eveniet voluptas molestias minus architecto perspiciatis natus voluptatem laboriosam temporibus quo fuga culpa odit. Lorem ipsum dolor sit amet consectetur adipisicing elit. Voluptatem, minus placeat? Quae, possimus alias! Perferendis, voluptates modi tempora quas hic unde libero totam in nulla ducimus dignissimos. Omnis, at iste.&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Ensina uma forma útil de usar o iframe, colocando links de sites que quando clicados é alterado o site no iframe</t>
+  </si>
+  <si>
+    <t>Acredito que pode ser feito com fotos também...</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +2255,12 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -1477,9 +2271,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,10 +2586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B80"/>
+  <dimension ref="A2:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +2746,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
@@ -1976,7 +2768,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="9"/>
+      <c r="B33" s="8"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
@@ -2002,7 +2794,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2046,13 +2838,13 @@
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
-      <c r="B47" s="9"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
@@ -2062,11 +2854,11 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
-      <c r="B49" s="9"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2098,13 +2890,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11"/>
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11"/>
-      <c r="B57" s="5"/>
+      <c r="B57" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
@@ -2112,95 +2906,181 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="B59" s="5"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
-      <c r="B60" s="5"/>
+      <c r="B60" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
-      <c r="B61" s="5"/>
+      <c r="B61" s="8"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
-      <c r="B62" s="5"/>
+      <c r="B62" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
-      <c r="B63" s="5"/>
+      <c r="B63" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
-      <c r="B64" s="5"/>
+      <c r="B64" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
-      <c r="B65" s="5"/>
+      <c r="B65" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
-      <c r="B66" s="5"/>
+      <c r="B66" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
-      <c r="B67" s="5"/>
+      <c r="B67" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
-      <c r="B68" s="5"/>
+      <c r="B68" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
-      <c r="B69" s="5"/>
+      <c r="B69" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
-      <c r="B70" s="5"/>
+      <c r="B70" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
-      <c r="B71" s="5"/>
+      <c r="B71" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
-      <c r="B72" s="5"/>
+      <c r="B72" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
-      <c r="B73" s="5"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
-      <c r="B74" s="5"/>
+      <c r="B74" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
-      <c r="B75" s="5"/>
+      <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
-      <c r="B76" s="5"/>
+      <c r="B76" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
-      <c r="B77" s="5"/>
+      <c r="B77" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
-      <c r="B78" s="5"/>
+      <c r="B78" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
-      <c r="B79" s="5"/>
-    </row>
-    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="7"/>
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
+      <c r="B80" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="11"/>
+      <c r="B82" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+      <c r="B83" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="11"/>
+      <c r="B84" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="12"/>
+      <c r="B91" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:A80"/>
+    <mergeCell ref="A5:A91"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado iframe003 e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E59F2D-62D2-427B-B91C-1D30C505AEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687E83A6-7D98-428C-B445-43E067E824EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
+    <workbookView xWindow="-28800" yWindow="135" windowWidth="14400" windowHeight="15750" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -2072,13 +2072,272 @@
   </si>
   <si>
     <t>Acredito que pode ser feito com fotos também...</t>
+  </si>
+  <si>
+    <t>Aula 5 – Conteúdo estático em iframe</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tela"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"frame"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>srcdoc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE96379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1&gt; Escolha uma das opções acima</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE96379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/h1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE96379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p&gt;Lorem ipsum, dolor sit amet consectetur adipisicing elit. 
+Quod quae quisquam, dolores libero ratione distinctio perspiciatis, numquam sit tenetur atque dolor similique, sapiente ducimus omnis reiciendis non! Quisquam, nobis natus? Lorem ipsum dolor sit amet consectetur adipisicing elit. Ab sapiente animi possimus tempore atque? Consectetur consequuntur accusamus, velit ea quaerat est vero ex quibusdam voluptatibus minus. Vitae, eum doloremque! Ea!</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE96379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/p&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE96379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img src='imagens/cursoemvideo.png'&gt; "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Ensina usar o srcdoc - Para colocar conteúdo html diretamente dentro do iframe. Não é uma opção muito legal de usar, mas serve de informação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2151,6 +2410,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFE96379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2262,6 +2529,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -2271,7 +2539,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2586,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B91"/>
+  <dimension ref="A2:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,7 +2876,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2617,470 +2884,518 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="8"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="8"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
+      <c r="A62" s="12"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
+      <c r="A63" s="12"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
+      <c r="A64" s="12"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
+      <c r="A65" s="12"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+      <c r="A67" s="12"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
+      <c r="A68" s="12"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
+      <c r="A69" s="12"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
+      <c r="A71" s="12"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+      <c r="A72" s="12"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
+      <c r="A73" s="12"/>
       <c r="B73" s="8"/>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
+      <c r="A74" s="12"/>
       <c r="B74" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
+      <c r="A75" s="12"/>
       <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+      <c r="A76" s="12"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+      <c r="A77" s="12"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+      <c r="A78" s="12"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
+      <c r="A79" s="12"/>
       <c r="B79" s="8"/>
     </row>
     <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
+      <c r="A80" s="12"/>
       <c r="B80" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="12"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="12"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="12"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+      <c r="A84" s="12"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+    <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="12"/>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86" s="3"/>
+    <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="12"/>
+      <c r="B86" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+      <c r="A87" s="12"/>
       <c r="B87" s="3"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
-      <c r="B88" s="3"/>
+    <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A88" s="12"/>
+      <c r="B88" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
-      <c r="B89" s="3"/>
+      <c r="A89" s="12"/>
+      <c r="B89" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="12"/>
+      <c r="B90" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
-      <c r="B91" s="13"/>
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="12"/>
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="12"/>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="12"/>
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="12"/>
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="12"/>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="12"/>
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="12"/>
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="12"/>
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="12"/>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="13"/>
+      <c r="B101" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:A91"/>
+    <mergeCell ref="A5:A101"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o iframe004 e pg004
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687E83A6-7D98-428C-B445-43E067E824EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251364A-AA84-4C0D-B31B-4D5CF324C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="135" windowWidth="14400" windowHeight="15750" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
+    <workbookView xWindow="-28800" yWindow="135" windowWidth="15810" windowHeight="15750" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -2331,6 +2331,146 @@
   </si>
   <si>
     <t>Ensina usar o srcdoc - Para colocar conteúdo html diretamente dentro do iframe. Não é uma opção muito legal de usar, mas serve de informação</t>
+  </si>
+  <si>
+    <t>Aula 7 – Tornando iframes mais seguros</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"paginas-extras/pag004.html"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sandbox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"allow-same-origin allow-forms allow-scripts"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>referrerpolicy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"no-referrer"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensina usar o sandbox e referrepolicy para melhorar a segurança do iframe...dúvidas assistir a aula novamente. </t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2538,6 +2678,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2853,10 +2996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B101"/>
+  <dimension ref="A2:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3349,13 +3492,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
-      <c r="B92" s="3"/>
+      <c r="B92" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
@@ -3363,7 +3508,9 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
-      <c r="B94" s="3"/>
+      <c r="B94" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
@@ -3371,11 +3518,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
-      <c r="B96" s="3"/>
+      <c r="B96" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
-      <c r="B97" s="3"/>
+      <c r="B97" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
@@ -3389,13 +3540,49 @@
       <c r="A100" s="12"/>
       <c r="B100" s="3"/>
     </row>
-    <row r="101" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="13"/>
-      <c r="B101" s="10"/>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="12"/>
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="12"/>
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="12"/>
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="12"/>
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="12"/>
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="12"/>
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="12"/>
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="12"/>
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="12"/>
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="13"/>
+      <c r="B110" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:A101"/>
+    <mergeCell ref="A5:A110"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criado o iframe006 e atualizado planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251364A-AA84-4C0D-B31B-4D5CF324C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122F3F9-A731-405A-A579-F49596FC46B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="135" windowWidth="15810" windowHeight="15750" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -2330,9 +2330,6 @@
     </r>
   </si>
   <si>
-    <t>Ensina usar o srcdoc - Para colocar conteúdo html diretamente dentro do iframe. Não é uma opção muito legal de usar, mas serve de informação</t>
-  </si>
-  <si>
     <t>Aula 7 – Tornando iframes mais seguros</t>
   </si>
   <si>
@@ -2471,6 +2468,22 @@
   </si>
   <si>
     <t xml:space="preserve">Ensina usar o sandbox e referrepolicy para melhorar a segurança do iframe...dúvidas assistir a aula novamente. </t>
+  </si>
+  <si>
+    <t>Ensina usar o srcdoc - Para colocar conteúdo html diretamente dentro do iframe. Não é uma opção muito legal de usar,
+ mas serve de informação</t>
+  </si>
+  <si>
+    <t>Aula 8 – Dicas interessantes para iframes</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5500/exercicios/ex024/iframe006.html</t>
+  </si>
+  <si>
+    <t>Ensina fazer vários tipos de incorporações utilizando iframes</t>
+  </si>
+  <si>
+    <t>Vídeos do vimeo, youtube, google maps, waze maps, google documents</t>
   </si>
 </sst>
 </file>
@@ -2644,7 +2657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2670,6 +2683,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -2679,8 +2695,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2996,10 +3012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B110"/>
+  <dimension ref="A2:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3019,7 +3035,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3027,562 +3043,550 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
+      <c r="A53" s="13"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="8"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+      <c r="A62" s="13"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
+      <c r="A63" s="13"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+      <c r="A64" s="13"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
+      <c r="A69" s="13"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
+      <c r="A70" s="13"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
+      <c r="A71" s="13"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
+      <c r="A72" s="13"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
+      <c r="A73" s="13"/>
       <c r="B73" s="8"/>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="12"/>
+      <c r="A76" s="13"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
+      <c r="A77" s="13"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="8"/>
     </row>
     <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
+      <c r="A80" s="13"/>
       <c r="B80" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
+      <c r="A81" s="13"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="12"/>
+      <c r="A82" s="13"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
+      <c r="A83" s="13"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
+      <c r="A84" s="13"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="12"/>
+      <c r="A85" s="13"/>
       <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="12"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
+      <c r="A88" s="13"/>
       <c r="B88" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="13"/>
       <c r="B89" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="5" t="s">
+    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+      <c r="B90" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="13"/>
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="13"/>
+      <c r="B92" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="12"/>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="12"/>
-      <c r="B92" s="6" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="13"/>
+      <c r="B94" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
-      <c r="B94" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
+      <c r="A95" s="13"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
+      <c r="A96" s="13"/>
       <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
+      <c r="A97" s="13"/>
       <c r="B97" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="13"/>
       <c r="B98" s="3"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="3"/>
+    <row r="99" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="13"/>
+      <c r="B99" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
+      <c r="A100" s="13"/>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="3"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
+      <c r="A102" s="13"/>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="12"/>
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="13"/>
-      <c r="B110" s="10"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="14"/>
+      <c r="B105" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:A110"/>
+    <mergeCell ref="A5:A105"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizada a planilha Cap24
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F41AF34-8AA2-44C1-AF5C-A0B5574DA00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28878366-D0B9-49F0-9728-4561A1138CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="217">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -10083,6 +10083,1119 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> para ele o Acesse em baixo da imagem e o resto já dá pra entender...</t>
+    </r>
+  </si>
+  <si>
+    <t>Capítulo 24</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Formulário&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>font-family</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Arial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Helvetica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sans-serif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Meu Primeiro Formulário&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"cadastro.php"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"off"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Nome:&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"nome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"isobrenome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Sobrenome: &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"sobrenome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"isobrenome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Enviar"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs.: </t>
+  </si>
+  <si>
+    <t>Um histórico de nomes já cadastrados no campo...</t>
+  </si>
+  <si>
+    <t>O name é mais útil para html e php. O id é mais útil para o javascript e é bom dar uma diferenciada no id com o i, tipo nome fica inome...</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toda tabela tem que ser feita dentro de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form e /form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">. O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>action cadastro php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para enviar os dados quando clicado no botão </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>submit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">. O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete off</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para não aparecer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No cadastro de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>nome e sobrenome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, coloca eles ente uma tag de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>parágrafo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e uma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>labe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">l e no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> coloca-se o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>nome ou o id do input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> para criar uma relação ou uma licação entre eles.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O Guanabara falou que usar </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é muito importante! Para fazer a relação de qual é o objeto de formulário e quel é a etiqueta dele e qual a relação entre um e outro!</t>
     </r>
   </si>
 </sst>
@@ -10090,7 +11203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10100,14 +11213,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -10212,6 +11317,21 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -10239,7 +11359,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -10299,62 +11419,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10671,10 +11830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B348"/>
+  <dimension ref="A2:B417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B352" sqref="B352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10694,1872 +11853,2200 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="9" t="s">
+      <c r="A46" s="14"/>
+      <c r="B46" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="8"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="9" t="s">
+      <c r="A50" s="14"/>
+      <c r="B50" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="14"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+      <c r="A54" s="14"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="18"/>
+      <c r="A56" s="14"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="9" t="s">
+      <c r="A60" s="14"/>
+      <c r="B60" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="8"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
+      <c r="A62" s="14"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
+      <c r="A63" s="14"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
+      <c r="A64" s="14"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
+      <c r="A65" s="14"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
+      <c r="A66" s="14"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
+      <c r="A68" s="14"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
+      <c r="A70" s="14"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+      <c r="A71" s="14"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
+      <c r="A72" s="14"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="18"/>
-      <c r="B73" s="8"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="7"/>
     </row>
     <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="18"/>
-      <c r="B74" s="9" t="s">
+      <c r="A74" s="14"/>
+      <c r="B74" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
-      <c r="B75" s="8"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
+      <c r="A76" s="14"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
+      <c r="A77" s="14"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="18"/>
+      <c r="A78" s="14"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
-      <c r="B79" s="8"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="7"/>
     </row>
     <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="18"/>
-      <c r="B80" s="9" t="s">
+      <c r="A80" s="14"/>
+      <c r="B80" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="18"/>
+      <c r="A81" s="14"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
+      <c r="A82" s="14"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
+      <c r="A83" s="14"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
+      <c r="A84" s="14"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="18"/>
+      <c r="A85" s="14"/>
       <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18"/>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
+      <c r="A87" s="14"/>
       <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="9" t="s">
+      <c r="A88" s="14"/>
+      <c r="B88" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
+      <c r="A89" s="14"/>
       <c r="B89" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
-      <c r="B90" s="12" t="s">
+      <c r="A90" s="14"/>
+      <c r="B90" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="18"/>
+      <c r="A91" s="14"/>
       <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="18"/>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="14"/>
+      <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="11" t="s">
+      <c r="A94" s="14"/>
+      <c r="B94" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
+      <c r="A95" s="14"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
+      <c r="A96" s="14"/>
       <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
+      <c r="A97" s="14"/>
       <c r="B97" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="18"/>
+      <c r="A98" s="14"/>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="18"/>
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="17" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
+      <c r="A100" s="14"/>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
+      <c r="A101" s="14"/>
       <c r="B101" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="18"/>
+      <c r="A102" s="14"/>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="18"/>
+      <c r="A103" s="14"/>
       <c r="B103" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="18"/>
+      <c r="A104" s="14"/>
       <c r="B104" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="19"/>
-      <c r="B105" s="10"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="9"/>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="17" t="s">
+      <c r="A109" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="18"/>
-      <c r="B110" s="13" t="s">
+      <c r="A110" s="14"/>
+      <c r="B110" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="18"/>
-      <c r="B111" s="11" t="s">
+      <c r="A111" s="14"/>
+      <c r="B111" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="18"/>
-      <c r="B112" s="11" t="s">
+      <c r="A112" s="14"/>
+      <c r="B112" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="18"/>
-      <c r="B113" s="11" t="s">
+      <c r="A113" s="14"/>
+      <c r="B113" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="18"/>
-      <c r="B114" s="11" t="s">
+      <c r="A114" s="14"/>
+      <c r="B114" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="18"/>
-      <c r="B115" s="11" t="s">
+      <c r="A115" s="14"/>
+      <c r="B115" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="18"/>
-      <c r="B116" s="11" t="s">
+      <c r="A116" s="14"/>
+      <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="18"/>
-      <c r="B117" s="11" t="s">
+      <c r="A117" s="14"/>
+      <c r="B117" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="18"/>
-      <c r="B118" s="11" t="s">
+      <c r="A118" s="14"/>
+      <c r="B118" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="18"/>
-      <c r="B119" s="11" t="s">
+      <c r="A119" s="14"/>
+      <c r="B119" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="18"/>
-      <c r="B120" s="11" t="s">
+      <c r="A120" s="14"/>
+      <c r="B120" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="18"/>
-      <c r="B121" s="11" t="s">
+      <c r="A121" s="14"/>
+      <c r="B121" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="18"/>
-      <c r="B122" s="11" t="s">
+      <c r="A122" s="14"/>
+      <c r="B122" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="18"/>
-      <c r="B123" s="11" t="s">
+      <c r="A123" s="14"/>
+      <c r="B123" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="18"/>
-      <c r="B124" s="11" t="s">
+      <c r="A124" s="14"/>
+      <c r="B124" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="18"/>
-      <c r="B125" s="11" t="s">
+      <c r="A125" s="14"/>
+      <c r="B125" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="18"/>
-      <c r="B126" s="11" t="s">
+      <c r="A126" s="14"/>
+      <c r="B126" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="18"/>
-      <c r="B127" s="11" t="s">
+      <c r="A127" s="14"/>
+      <c r="B127" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="18"/>
-      <c r="B128" s="11" t="s">
+      <c r="A128" s="14"/>
+      <c r="B128" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="18"/>
-      <c r="B129" s="11" t="s">
+      <c r="A129" s="14"/>
+      <c r="B129" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="18"/>
-      <c r="B130" s="11" t="s">
+      <c r="A130" s="14"/>
+      <c r="B130" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="18"/>
-      <c r="B131" s="11" t="s">
+      <c r="A131" s="14"/>
+      <c r="B131" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="18"/>
-      <c r="B132" s="11" t="s">
+      <c r="A132" s="14"/>
+      <c r="B132" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="18"/>
-      <c r="B133" s="11" t="s">
+      <c r="A133" s="14"/>
+      <c r="B133" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="18"/>
-      <c r="B134" s="11" t="s">
+      <c r="A134" s="14"/>
+      <c r="B134" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="18"/>
-      <c r="B135" s="11" t="s">
+      <c r="A135" s="14"/>
+      <c r="B135" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="18"/>
-      <c r="B136" s="11" t="s">
+      <c r="A136" s="14"/>
+      <c r="B136" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="18"/>
-      <c r="B137" s="11" t="s">
+      <c r="A137" s="14"/>
+      <c r="B137" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="18"/>
+      <c r="A138" s="14"/>
       <c r="B138" s="3"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="18"/>
+      <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="18"/>
+      <c r="A140" s="14"/>
       <c r="B140" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="18"/>
+      <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="18"/>
-      <c r="B142" s="16" t="s">
+      <c r="A142" s="14"/>
+      <c r="B142" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="18"/>
-      <c r="B143" s="16" t="s">
+      <c r="A143" s="14"/>
+      <c r="B143" s="13" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="18"/>
-      <c r="B144" s="16" t="s">
+      <c r="A144" s="14"/>
+      <c r="B144" s="13" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="18"/>
+      <c r="A145" s="14"/>
       <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="18"/>
-      <c r="B146" s="13" t="s">
+      <c r="A146" s="14"/>
+      <c r="B146" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="18"/>
+      <c r="A147" s="14"/>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="18"/>
-      <c r="B148" s="11" t="s">
+      <c r="A148" s="14"/>
+      <c r="B148" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="18"/>
-      <c r="B149" s="11" t="s">
+      <c r="A149" s="14"/>
+      <c r="B149" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="18"/>
-      <c r="B150" s="11" t="s">
+      <c r="A150" s="14"/>
+      <c r="B150" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="18"/>
-      <c r="B151" s="11" t="s">
+      <c r="A151" s="14"/>
+      <c r="B151" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="18"/>
-      <c r="B152" s="11" t="s">
+      <c r="A152" s="14"/>
+      <c r="B152" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="18"/>
-      <c r="B153" s="11" t="s">
+      <c r="A153" s="14"/>
+      <c r="B153" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="18"/>
-      <c r="B154" s="11" t="s">
+      <c r="A154" s="14"/>
+      <c r="B154" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="18"/>
-      <c r="B155" s="11" t="s">
+      <c r="A155" s="14"/>
+      <c r="B155" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="18"/>
-      <c r="B156" s="11" t="s">
+      <c r="A156" s="14"/>
+      <c r="B156" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="18"/>
-      <c r="B157" s="11" t="s">
+      <c r="A157" s="14"/>
+      <c r="B157" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="18"/>
-      <c r="B158" s="11" t="s">
+      <c r="A158" s="14"/>
+      <c r="B158" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="18"/>
-      <c r="B159" s="11" t="s">
+      <c r="A159" s="14"/>
+      <c r="B159" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="18"/>
-      <c r="B160" s="14"/>
+      <c r="A160" s="14"/>
+      <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="18"/>
-      <c r="B161" s="11" t="s">
+      <c r="A161" s="14"/>
+      <c r="B161" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="18"/>
-      <c r="B162" s="11" t="s">
+      <c r="A162" s="14"/>
+      <c r="B162" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="18"/>
-      <c r="B163" s="11" t="s">
+      <c r="A163" s="14"/>
+      <c r="B163" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="18"/>
-      <c r="B164" s="11" t="s">
+      <c r="A164" s="14"/>
+      <c r="B164" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="18"/>
-      <c r="B165" s="11" t="s">
+      <c r="A165" s="14"/>
+      <c r="B165" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="18"/>
-      <c r="B166" s="11" t="s">
+      <c r="A166" s="14"/>
+      <c r="B166" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="18"/>
-      <c r="B167" s="11" t="s">
+      <c r="A167" s="14"/>
+      <c r="B167" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="18"/>
-      <c r="B168" s="11" t="s">
+      <c r="A168" s="14"/>
+      <c r="B168" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="18"/>
-      <c r="B169" s="11" t="s">
+      <c r="A169" s="14"/>
+      <c r="B169" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="18"/>
-      <c r="B170" s="11" t="s">
+      <c r="A170" s="14"/>
+      <c r="B170" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="18"/>
-      <c r="B171" s="11" t="s">
+      <c r="A171" s="14"/>
+      <c r="B171" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="18"/>
+      <c r="A172" s="14"/>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="18"/>
+      <c r="A173" s="14"/>
       <c r="B173" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="18"/>
+      <c r="A174" s="14"/>
       <c r="B174" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="18"/>
+      <c r="A175" s="14"/>
       <c r="B175" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="18"/>
+      <c r="A176" s="14"/>
       <c r="B176" s="5"/>
     </row>
     <row r="177" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="18"/>
-      <c r="B177" s="13" t="s">
+      <c r="A177" s="14"/>
+      <c r="B177" s="12" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="18"/>
+      <c r="A178" s="14"/>
       <c r="B178" s="5"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="18"/>
-      <c r="B179" s="11" t="s">
+      <c r="A179" s="14"/>
+      <c r="B179" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="18"/>
-      <c r="B180" s="11" t="s">
+      <c r="A180" s="14"/>
+      <c r="B180" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="18"/>
-      <c r="B181" s="11" t="s">
+      <c r="A181" s="14"/>
+      <c r="B181" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="18"/>
-      <c r="B182" s="11" t="s">
+      <c r="A182" s="14"/>
+      <c r="B182" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="18"/>
-      <c r="B183" s="11" t="s">
+      <c r="A183" s="14"/>
+      <c r="B183" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="18"/>
-      <c r="B184" s="11" t="s">
+      <c r="A184" s="14"/>
+      <c r="B184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="18"/>
-      <c r="B185" s="11" t="s">
+      <c r="A185" s="14"/>
+      <c r="B185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="18"/>
-      <c r="B186" s="11" t="s">
+      <c r="A186" s="14"/>
+      <c r="B186" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="18"/>
-      <c r="B187" s="11" t="s">
+      <c r="A187" s="14"/>
+      <c r="B187" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="18"/>
-      <c r="B188" s="11" t="s">
+      <c r="A188" s="14"/>
+      <c r="B188" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="18"/>
-      <c r="B189" s="11" t="s">
+      <c r="A189" s="14"/>
+      <c r="B189" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="18"/>
-      <c r="B190" s="11" t="s">
+      <c r="A190" s="14"/>
+      <c r="B190" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="18"/>
-      <c r="B191" s="11" t="s">
+      <c r="A191" s="14"/>
+      <c r="B191" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="18"/>
+      <c r="A192" s="14"/>
       <c r="B192" s="5"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="18"/>
+      <c r="A193" s="14"/>
       <c r="B193" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="18"/>
+      <c r="A194" s="14"/>
       <c r="B194" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="18"/>
+      <c r="A195" s="14"/>
       <c r="B195" s="5"/>
     </row>
     <row r="196" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="18"/>
-      <c r="B196" s="13" t="s">
+      <c r="A196" s="14"/>
+      <c r="B196" s="12" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="18"/>
-      <c r="B197" s="5"/>
+      <c r="A197" s="14"/>
+      <c r="B197" s="20"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="18"/>
-      <c r="B198" s="15" t="s">
+      <c r="A198" s="14"/>
+      <c r="B198" s="19" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="18"/>
-      <c r="B199" s="14"/>
+      <c r="A199" s="14"/>
+      <c r="B199" s="7"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="18"/>
-      <c r="B200" s="15" t="s">
+      <c r="A200" s="14"/>
+      <c r="B200" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="18"/>
-      <c r="B201" s="11" t="s">
+      <c r="A201" s="14"/>
+      <c r="B201" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="18"/>
-      <c r="B202" s="11" t="s">
+      <c r="A202" s="14"/>
+      <c r="B202" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="18"/>
-      <c r="B203" s="11" t="s">
+      <c r="A203" s="14"/>
+      <c r="B203" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="18"/>
-      <c r="B204" s="11" t="s">
+      <c r="A204" s="14"/>
+      <c r="B204" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="18"/>
-      <c r="B205" s="20" t="s">
+      <c r="A205" s="14"/>
+      <c r="B205" s="21" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="18"/>
-      <c r="B206" s="11" t="s">
+      <c r="A206" s="14"/>
+      <c r="B206" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="18"/>
-      <c r="B207" s="11" t="s">
+      <c r="A207" s="14"/>
+      <c r="B207" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="18"/>
-      <c r="B208" s="11" t="s">
+      <c r="A208" s="14"/>
+      <c r="B208" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="18"/>
-      <c r="B209" s="11" t="s">
+      <c r="A209" s="14"/>
+      <c r="B209" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="18"/>
-      <c r="B210" s="15" t="s">
+      <c r="A210" s="14"/>
+      <c r="B210" s="19" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="18"/>
-      <c r="B211" s="11" t="s">
+      <c r="A211" s="14"/>
+      <c r="B211" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="18"/>
-      <c r="B212" s="11" t="s">
+      <c r="A212" s="14"/>
+      <c r="B212" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="18"/>
-      <c r="B213" s="14"/>
+      <c r="A213" s="14"/>
+      <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="18"/>
-      <c r="B214" s="15" t="s">
+      <c r="A214" s="14"/>
+      <c r="B214" s="19" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="18"/>
-      <c r="B215" s="11" t="s">
+      <c r="A215" s="14"/>
+      <c r="B215" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="18"/>
-      <c r="B216" s="11" t="s">
+      <c r="A216" s="14"/>
+      <c r="B216" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="18"/>
-      <c r="B217" s="11" t="s">
+      <c r="A217" s="14"/>
+      <c r="B217" s="3" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="18"/>
-      <c r="B218" s="11" t="s">
+      <c r="A218" s="14"/>
+      <c r="B218" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="18"/>
-      <c r="B219" s="11" t="s">
+      <c r="A219" s="14"/>
+      <c r="B219" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="18"/>
-      <c r="B220" s="11" t="s">
+      <c r="A220" s="14"/>
+      <c r="B220" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="18"/>
-      <c r="B221" s="11" t="s">
+      <c r="A221" s="14"/>
+      <c r="B221" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="18"/>
-      <c r="B222" s="14"/>
+      <c r="A222" s="14"/>
+      <c r="B222" s="7"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="18"/>
-      <c r="B223" s="15" t="s">
+      <c r="A223" s="14"/>
+      <c r="B223" s="19" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="18"/>
-      <c r="B224" s="11" t="s">
+      <c r="A224" s="14"/>
+      <c r="B224" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="18"/>
-      <c r="B225" s="11" t="s">
+      <c r="A225" s="14"/>
+      <c r="B225" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="18"/>
+      <c r="A226" s="14"/>
       <c r="B226" s="5"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="18"/>
+      <c r="A227" s="14"/>
       <c r="B227" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="18"/>
+      <c r="A228" s="14"/>
       <c r="B228" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="18"/>
+      <c r="A229" s="14"/>
       <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="18"/>
-      <c r="B230" s="13" t="s">
+      <c r="A230" s="14"/>
+      <c r="B230" s="12" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="18"/>
+      <c r="A231" s="14"/>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="18"/>
-      <c r="B232" s="15" t="s">
+      <c r="A232" s="14"/>
+      <c r="B232" s="19" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="18"/>
-      <c r="B233" s="14"/>
+      <c r="A233" s="14"/>
+      <c r="B233" s="7"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="18"/>
-      <c r="B234" s="15" t="s">
+      <c r="A234" s="14"/>
+      <c r="B234" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="18"/>
-      <c r="B235" s="11" t="s">
+      <c r="A235" s="14"/>
+      <c r="B235" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="18"/>
-      <c r="B236" s="11" t="s">
+      <c r="A236" s="14"/>
+      <c r="B236" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="18"/>
-      <c r="B237" s="11" t="s">
+      <c r="A237" s="14"/>
+      <c r="B237" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="18"/>
-      <c r="B238" s="11" t="s">
+      <c r="A238" s="14"/>
+      <c r="B238" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="18"/>
-      <c r="B239" s="14"/>
+      <c r="A239" s="14"/>
+      <c r="B239" s="7"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="18"/>
-      <c r="B240" s="15" t="s">
+      <c r="A240" s="14"/>
+      <c r="B240" s="19" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="18"/>
-      <c r="B241" s="11" t="s">
+      <c r="A241" s="14"/>
+      <c r="B241" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="18"/>
-      <c r="B242" s="11" t="s">
+      <c r="A242" s="14"/>
+      <c r="B242" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="18"/>
-      <c r="B243" s="11" t="s">
+      <c r="A243" s="14"/>
+      <c r="B243" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="18"/>
-      <c r="B244" s="11" t="s">
+      <c r="A244" s="14"/>
+      <c r="B244" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="18"/>
-      <c r="B245" s="14"/>
+      <c r="A245" s="14"/>
+      <c r="B245" s="7"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="18"/>
-      <c r="B246" s="15" t="s">
+      <c r="A246" s="14"/>
+      <c r="B246" s="19" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="18"/>
-      <c r="B247" s="11" t="s">
+      <c r="A247" s="14"/>
+      <c r="B247" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="18"/>
-      <c r="B248" s="11" t="s">
+      <c r="A248" s="14"/>
+      <c r="B248" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="18"/>
-      <c r="B249" s="11" t="s">
+      <c r="A249" s="14"/>
+      <c r="B249" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="18"/>
-      <c r="B250" s="11" t="s">
+      <c r="A250" s="14"/>
+      <c r="B250" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="18"/>
-      <c r="B251" s="14"/>
+      <c r="A251" s="14"/>
+      <c r="B251" s="7"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="18"/>
-      <c r="B252" s="15" t="s">
+      <c r="A252" s="14"/>
+      <c r="B252" s="19" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="18"/>
-      <c r="B253" s="11" t="s">
+      <c r="A253" s="14"/>
+      <c r="B253" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="18"/>
-      <c r="B254" s="11" t="s">
+      <c r="A254" s="14"/>
+      <c r="B254" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="18"/>
-      <c r="B255" s="11" t="s">
+      <c r="A255" s="14"/>
+      <c r="B255" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="18"/>
-      <c r="B256" s="14"/>
+      <c r="A256" s="14"/>
+      <c r="B256" s="7"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="18"/>
-      <c r="B257" s="15" t="s">
+      <c r="A257" s="14"/>
+      <c r="B257" s="19" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="18"/>
-      <c r="B258" s="11" t="s">
+      <c r="A258" s="14"/>
+      <c r="B258" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="18"/>
-      <c r="B259" s="11" t="s">
+      <c r="A259" s="14"/>
+      <c r="B259" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="18"/>
-      <c r="B260" s="11" t="s">
+      <c r="A260" s="14"/>
+      <c r="B260" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="18"/>
-      <c r="B261" s="11" t="s">
+      <c r="A261" s="14"/>
+      <c r="B261" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="18"/>
-      <c r="B262" s="11" t="s">
+      <c r="A262" s="14"/>
+      <c r="B262" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="18"/>
-      <c r="B263" s="11" t="s">
+      <c r="A263" s="14"/>
+      <c r="B263" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="18"/>
-      <c r="B264" s="11" t="s">
+      <c r="A264" s="14"/>
+      <c r="B264" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="18"/>
-      <c r="B265" s="11" t="s">
+      <c r="A265" s="14"/>
+      <c r="B265" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="18"/>
-      <c r="B266" s="14"/>
+      <c r="A266" s="14"/>
+      <c r="B266" s="7"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="18"/>
-      <c r="B267" s="15" t="s">
+      <c r="A267" s="14"/>
+      <c r="B267" s="19" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="18"/>
-      <c r="B268" s="11" t="s">
+      <c r="A268" s="14"/>
+      <c r="B268" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="18"/>
-      <c r="B269" s="11" t="s">
+      <c r="A269" s="14"/>
+      <c r="B269" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="18"/>
-      <c r="B270" s="11" t="s">
+      <c r="A270" s="14"/>
+      <c r="B270" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="18"/>
-      <c r="B271" s="11" t="s">
+      <c r="A271" s="14"/>
+      <c r="B271" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="18"/>
-      <c r="B272" s="11" t="s">
+      <c r="A272" s="14"/>
+      <c r="B272" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="18"/>
-      <c r="B273" s="11" t="s">
+      <c r="A273" s="14"/>
+      <c r="B273" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="18"/>
-      <c r="B274" s="14"/>
+      <c r="A274" s="14"/>
+      <c r="B274" s="7"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="18"/>
-      <c r="B275" s="15" t="s">
+      <c r="A275" s="14"/>
+      <c r="B275" s="19" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="18"/>
-      <c r="B276" s="11" t="s">
+      <c r="A276" s="14"/>
+      <c r="B276" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="18"/>
-      <c r="B277" s="11" t="s">
+      <c r="A277" s="14"/>
+      <c r="B277" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="18"/>
-      <c r="B278" s="14"/>
+      <c r="A278" s="14"/>
+      <c r="B278" s="7"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="18"/>
-      <c r="B279" s="15" t="s">
+      <c r="A279" s="14"/>
+      <c r="B279" s="19" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="18"/>
-      <c r="B280" s="11" t="s">
+      <c r="A280" s="14"/>
+      <c r="B280" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="18"/>
-      <c r="B281" s="11" t="s">
+      <c r="A281" s="14"/>
+      <c r="B281" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="18"/>
-      <c r="B282" s="11" t="s">
+      <c r="A282" s="14"/>
+      <c r="B282" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="18"/>
-      <c r="B283" s="11" t="s">
+      <c r="A283" s="14"/>
+      <c r="B283" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="18"/>
-      <c r="B284" s="11" t="s">
+      <c r="A284" s="14"/>
+      <c r="B284" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="18"/>
-      <c r="B285" s="11" t="s">
+      <c r="A285" s="14"/>
+      <c r="B285" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="18"/>
-      <c r="B286" s="14"/>
+      <c r="A286" s="14"/>
+      <c r="B286" s="7"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="18"/>
-      <c r="B287" s="15" t="s">
+      <c r="A287" s="14"/>
+      <c r="B287" s="19" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="18"/>
-      <c r="B288" s="11" t="s">
+      <c r="A288" s="14"/>
+      <c r="B288" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="18"/>
-      <c r="B289" s="11" t="s">
+      <c r="A289" s="14"/>
+      <c r="B289" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="18"/>
-      <c r="B290" s="11" t="s">
+      <c r="A290" s="14"/>
+      <c r="B290" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="18"/>
-      <c r="B291" s="11" t="s">
+      <c r="A291" s="14"/>
+      <c r="B291" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="18"/>
-      <c r="B292" s="11" t="s">
+      <c r="A292" s="14"/>
+      <c r="B292" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="18"/>
+      <c r="A293" s="14"/>
       <c r="B293" s="5"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="18"/>
+      <c r="A294" s="14"/>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="18"/>
+      <c r="A295" s="14"/>
       <c r="B295" s="5"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="18"/>
-      <c r="B296" s="5"/>
+      <c r="A296" s="14"/>
+      <c r="B296" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="18"/>
-      <c r="B297" s="5"/>
+      <c r="A297" s="14"/>
+      <c r="B297" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="18"/>
-      <c r="B298" s="5"/>
+      <c r="A298" s="14"/>
+      <c r="B298" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="18"/>
-      <c r="B299" s="5"/>
+      <c r="A299" s="14"/>
+      <c r="B299" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="18"/>
-      <c r="B300" s="5"/>
+      <c r="A300" s="14"/>
+      <c r="B300" s="5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="18"/>
-      <c r="B301" s="5"/>
+      <c r="A301" s="14"/>
+      <c r="B301" s="5" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="18"/>
-      <c r="B302" s="5"/>
+      <c r="A302" s="14"/>
+      <c r="B302" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="18"/>
-      <c r="B303" s="5"/>
+      <c r="A303" s="14"/>
+      <c r="B303" s="5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="18"/>
-      <c r="B304" s="5"/>
+      <c r="A304" s="14"/>
+      <c r="B304" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="18"/>
-      <c r="B305" s="5"/>
+      <c r="A305" s="14"/>
+      <c r="B305" s="5" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="18"/>
-      <c r="B306" s="5"/>
+      <c r="A306" s="14"/>
+      <c r="B306" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="18"/>
-      <c r="B307" s="5"/>
+      <c r="A307" s="14"/>
+      <c r="B307" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="18"/>
-      <c r="B308" s="5"/>
+      <c r="A308" s="14"/>
+      <c r="B308" s="5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="18"/>
-      <c r="B309" s="5"/>
+      <c r="A309" s="14"/>
+      <c r="B309" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="18"/>
+      <c r="A310" s="14"/>
       <c r="B310" s="5" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="18"/>
+      <c r="A311" s="14"/>
       <c r="B311" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="18"/>
-      <c r="B312" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="18"/>
-      <c r="B313" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="18"/>
-      <c r="B314" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="18"/>
-      <c r="B315" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="18"/>
-      <c r="B316" s="5" t="s">
-        <v>154</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A312" s="15"/>
+      <c r="B312" s="9"/>
+    </row>
+    <row r="315" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="316" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B316" s="17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="18"/>
-      <c r="B317" s="5" t="s">
-        <v>155</v>
-      </c>
+      <c r="A317" s="14"/>
+      <c r="B317" s="1"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="18"/>
-      <c r="B318" s="5" t="s">
-        <v>156</v>
-      </c>
+      <c r="A318" s="14"/>
+      <c r="B318" s="3"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="18"/>
-      <c r="B319" s="5" t="s">
-        <v>157</v>
-      </c>
+      <c r="A319" s="14"/>
+      <c r="B319" s="2"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="18"/>
-      <c r="B320" s="5" t="s">
-        <v>158</v>
+      <c r="A320" s="14"/>
+      <c r="B320" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="18"/>
-      <c r="B321" s="5" t="s">
-        <v>159</v>
+      <c r="A321" s="14"/>
+      <c r="B321" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="18"/>
-      <c r="B322" s="5" t="s">
-        <v>160</v>
+      <c r="A322" s="14"/>
+      <c r="B322" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="18"/>
-      <c r="B323" s="5" t="s">
-        <v>162</v>
+      <c r="A323" s="14"/>
+      <c r="B323" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="18"/>
-      <c r="B324" s="5" t="s">
-        <v>163</v>
+      <c r="A324" s="14"/>
+      <c r="B324" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="18"/>
-      <c r="B325" s="5" t="s">
-        <v>164</v>
+      <c r="A325" s="14"/>
+      <c r="B325" s="10" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="18"/>
-      <c r="B326" s="5"/>
+      <c r="A326" s="14"/>
+      <c r="B326" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="18"/>
-      <c r="B327" s="5"/>
+      <c r="B327" s="10" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="18"/>
-      <c r="B328" s="5"/>
+      <c r="A328" s="14"/>
+      <c r="B328" s="10" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="18"/>
-      <c r="B329" s="5"/>
+      <c r="A329" s="14"/>
+      <c r="B329" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="18"/>
-      <c r="B330" s="5"/>
+      <c r="A330" s="14"/>
+      <c r="B330" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="18"/>
-      <c r="B331" s="5"/>
+      <c r="A331" s="14"/>
+      <c r="B331" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="18"/>
-      <c r="B332" s="5"/>
+      <c r="A332" s="14"/>
+      <c r="B332" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="18"/>
-      <c r="B333" s="5"/>
+      <c r="A333" s="14"/>
+      <c r="B333" s="10" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="18"/>
-      <c r="B334" s="5"/>
+      <c r="A334" s="14"/>
+      <c r="B334" s="10" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="18"/>
-      <c r="B335" s="5"/>
+      <c r="A335" s="14"/>
+      <c r="B335" s="10" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="18"/>
-      <c r="B336" s="5"/>
+      <c r="A336" s="14"/>
+      <c r="B336" s="10" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="18"/>
-      <c r="B337" s="5"/>
+      <c r="A337" s="14"/>
+      <c r="B337" s="10" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="18"/>
-      <c r="B338" s="3"/>
+      <c r="A338" s="14"/>
+      <c r="B338" s="10" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="18"/>
-      <c r="B339" s="5"/>
+      <c r="A339" s="14"/>
+      <c r="B339" s="10" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="18"/>
-      <c r="B340" s="5"/>
+      <c r="A340" s="14"/>
+      <c r="B340" s="10" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="18"/>
-      <c r="B341" s="3"/>
+      <c r="A341" s="14"/>
+      <c r="B341" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="18"/>
-      <c r="B342" s="5"/>
+      <c r="A342" s="14"/>
+      <c r="B342" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="18"/>
+      <c r="A343" s="14"/>
       <c r="B343" s="3"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="18"/>
-      <c r="B344" s="3"/>
+      <c r="A344" s="14"/>
+      <c r="B344" s="7"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="18"/>
+      <c r="A345" s="14"/>
       <c r="B345" s="3"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="18"/>
+      <c r="A346" s="14"/>
       <c r="B346" s="3"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="18"/>
-      <c r="B347" s="3"/>
-    </row>
-    <row r="348" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A348" s="19"/>
-      <c r="B348" s="10"/>
+      <c r="A347" s="14"/>
+      <c r="B347" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="14"/>
+      <c r="B348" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="14"/>
+      <c r="B349" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="14"/>
+      <c r="B350" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="14"/>
+      <c r="B351" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="14"/>
+      <c r="B352" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="14"/>
+      <c r="B353" s="5"/>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="18"/>
+      <c r="B354" s="3"/>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="14"/>
+      <c r="B355" s="5"/>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="14"/>
+      <c r="B356" s="3"/>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="14"/>
+      <c r="B357" s="3"/>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="14"/>
+      <c r="B358" s="8"/>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="14"/>
+      <c r="B359" s="7"/>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="14"/>
+      <c r="B360" s="3"/>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="14"/>
+      <c r="B361" s="7"/>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="14"/>
+      <c r="B362" s="8"/>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="14"/>
+      <c r="B363" s="3"/>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="14"/>
+      <c r="B364" s="5"/>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="14"/>
+      <c r="B365" s="5"/>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="14"/>
+      <c r="B366" s="5"/>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="14"/>
+      <c r="B367" s="5"/>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="14"/>
+      <c r="B368" s="5"/>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="18"/>
+      <c r="B369" s="3"/>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="14"/>
+      <c r="B370" s="5"/>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="14"/>
+      <c r="B371" s="3"/>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="14"/>
+      <c r="B372" s="8"/>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="14"/>
+      <c r="B373" s="7"/>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="14"/>
+      <c r="B374" s="3"/>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="14"/>
+      <c r="B375" s="3"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="14"/>
+      <c r="B376" s="3"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="14"/>
+      <c r="B377" s="3"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="14"/>
+      <c r="B378" s="3"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="14"/>
+      <c r="B379" s="3"/>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="14"/>
+      <c r="B380" s="3"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="14"/>
+      <c r="B381" s="3"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="14"/>
+      <c r="B382" s="3"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="14"/>
+      <c r="B383" s="3"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="14"/>
+      <c r="B384" s="3"/>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="14"/>
+      <c r="B385" s="7"/>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="14"/>
+      <c r="B386" s="8"/>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="14"/>
+      <c r="B387" s="7"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="14"/>
+      <c r="B388" s="3"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" s="14"/>
+      <c r="B389" s="3"/>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" s="14"/>
+      <c r="B390" s="3"/>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" s="14"/>
+      <c r="B391" s="7"/>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" s="14"/>
+      <c r="B392" s="8"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" s="14"/>
+      <c r="B393" s="3"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" s="14"/>
+      <c r="B394" s="5"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" s="14"/>
+      <c r="B395" s="5"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" s="14"/>
+      <c r="B396" s="5"/>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" s="14"/>
+      <c r="B397" s="3"/>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" s="18"/>
+      <c r="B398" s="3"/>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" s="14"/>
+      <c r="B399" s="3"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" s="14"/>
+      <c r="B400" s="8"/>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="14"/>
+      <c r="B401" s="5"/>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="14"/>
+      <c r="B402" s="11"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="14"/>
+      <c r="B403" s="3"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="18"/>
+      <c r="B404" s="3"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="14"/>
+      <c r="B405" s="3"/>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="14"/>
+      <c r="B406" s="3"/>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="14"/>
+      <c r="B407" s="3"/>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="14"/>
+      <c r="B408" s="5"/>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="14"/>
+      <c r="B409" s="5"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="14"/>
+      <c r="B410" s="3"/>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="18"/>
+      <c r="B411" s="3"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="14"/>
+      <c r="B412" s="3"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="14"/>
+      <c r="B413" s="3"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="14"/>
+      <c r="B414" s="3"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="14"/>
+      <c r="B415" s="3"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="14"/>
+      <c r="B416" s="3"/>
+    </row>
+    <row r="417" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A417" s="15"/>
+      <c r="B417" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A5:A105"/>
-    <mergeCell ref="A109:A348"/>
+    <mergeCell ref="A109:A312"/>
+    <mergeCell ref="A316:A417"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizada a planilha - method GET e POST
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28878366-D0B9-49F0-9728-4561A1138CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BFB793-A488-4CC0-95A8-C8D423F4A35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="225">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -11196,6 +11196,455 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> é muito importante! Para fazer a relação de qual é o objeto de formulário e quel é a etiqueta dele e qual a relação entre um e outro!</t>
+    </r>
+  </si>
+  <si>
+    <t>Capítulo 24 - Aula 1 e 2 - Criando e aprimorando formulários com label</t>
+  </si>
+  <si>
+    <t>Aula 3 – Métodos GET e POST</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O html têm 2 métodos simples para envio de formulário: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, sendo o </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>GET usado como padrão</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> se não for informato o padrão na tag form</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>GET tem um problema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> que quando envia o formulário, os dados dos inputs aparecem na URL da página. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Já o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>POS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">T não aparece na URL.  Mas não quer dizer que é mais seguro, pois conforme abaixo, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>os dados ficam expostos no devtools/network/headers/formdata....</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Por conta de ser o http... Para resolver o problema é necessário usar o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>...mais é mais avançado e veremos isso futuramente para enviar dados de cpf e cartão de crédito</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se usa o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dados NÂO sensíveis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> como: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nome, peso, idade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">... Ou </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coisas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">são </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secretas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, para links compartilháveis... </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Para dados </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">menores </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>que 3kb ou 3.000 letras</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de dados do form inteiro,  e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>envio de arquivos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>..</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se usa o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> para </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dados sensíveis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, se os dados tiver </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>mais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> que </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3 mil bites(3kb) e enviar qualquer tipo de arquivo, anexo ou foto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>. E os dois têm a mesma performance.</t>
     </r>
   </si>
 </sst>
@@ -11203,7 +11652,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11332,6 +11781,29 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -11456,7 +11928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -11489,20 +11961,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -11514,6 +11974,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -11531,6 +12006,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>44822</xdr:colOff>
+      <xdr:row>362</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12209945</xdr:colOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>49033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4482A715-C956-3C4E-146D-9D8D68653A01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="649940" y="72412411"/>
+          <a:ext cx="12165123" cy="6077798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11832,8 +12356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
   <dimension ref="A2:B417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B352" sqref="B352"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11853,2193 +12377,2207 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
-      <c r="B42" s="17" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="18"/>
-      <c r="B57" s="17" t="s">
+      <c r="A57" s="21"/>
+      <c r="B57" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="20"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="20"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="20"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="20"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+      <c r="A67" s="20"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="20"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="7"/>
     </row>
     <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="20"/>
       <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="20"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
+      <c r="A78" s="20"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="20"/>
       <c r="B79" s="7"/>
     </row>
     <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="20"/>
       <c r="B80" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="20"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="20"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="20"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="20"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="14"/>
+      <c r="A85" s="20"/>
       <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="18"/>
-      <c r="B86" s="17" t="s">
+      <c r="A86" s="21"/>
+      <c r="B86" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="20"/>
       <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
+      <c r="A88" s="20"/>
       <c r="B88" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="20"/>
       <c r="B89" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="20"/>
       <c r="B90" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="14"/>
+      <c r="A91" s="20"/>
       <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="18"/>
-      <c r="B92" s="17" t="s">
+      <c r="A92" s="21"/>
+      <c r="B92" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
+      <c r="A93" s="20"/>
       <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="20"/>
       <c r="B94" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="20"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="20"/>
       <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="20"/>
       <c r="B97" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="14"/>
+      <c r="A98" s="20"/>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="18"/>
-      <c r="B99" s="17" t="s">
+      <c r="A99" s="21"/>
+      <c r="B99" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="20"/>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
+      <c r="A101" s="20"/>
       <c r="B101" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="20"/>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="20"/>
       <c r="B103" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="20"/>
       <c r="B104" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="15"/>
+      <c r="A105" s="22"/>
       <c r="B105" s="9"/>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="16" t="s">
+      <c r="A109" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B109" s="17" t="s">
+      <c r="B109" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="14"/>
+      <c r="A110" s="20"/>
       <c r="B110" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
+      <c r="A111" s="20"/>
       <c r="B111" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
+      <c r="A112" s="20"/>
       <c r="B112" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="20"/>
       <c r="B113" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
+      <c r="A114" s="20"/>
       <c r="B114" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="20"/>
       <c r="B115" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="20"/>
       <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
+      <c r="A117" s="20"/>
       <c r="B117" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="20"/>
       <c r="B118" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="20"/>
       <c r="B119" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="20"/>
       <c r="B120" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="20"/>
       <c r="B121" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="20"/>
       <c r="B122" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
+      <c r="A123" s="20"/>
       <c r="B123" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="20"/>
       <c r="B124" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="20"/>
       <c r="B125" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
+      <c r="A126" s="20"/>
       <c r="B126" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="20"/>
       <c r="B127" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="14"/>
+      <c r="A128" s="20"/>
       <c r="B128" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="20"/>
       <c r="B129" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="20"/>
       <c r="B130" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="20"/>
       <c r="B131" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="20"/>
       <c r="B132" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="20"/>
       <c r="B133" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="14"/>
+      <c r="A134" s="20"/>
       <c r="B134" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="20"/>
       <c r="B135" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="20"/>
       <c r="B136" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="20"/>
       <c r="B137" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="20"/>
       <c r="B138" s="3"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="20"/>
       <c r="B139" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="20"/>
       <c r="B140" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="20"/>
       <c r="B141" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="20"/>
       <c r="B142" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="20"/>
       <c r="B143" s="13" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="14"/>
+      <c r="A144" s="20"/>
       <c r="B144" s="13" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="14"/>
+      <c r="A145" s="20"/>
       <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="14"/>
+      <c r="A146" s="20"/>
       <c r="B146" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="20"/>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="20"/>
       <c r="B148" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="14"/>
+      <c r="A149" s="20"/>
       <c r="B149" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="20"/>
       <c r="B150" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="20"/>
       <c r="B151" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="20"/>
       <c r="B152" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="20"/>
       <c r="B153" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="20"/>
       <c r="B154" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="20"/>
       <c r="B155" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="20"/>
       <c r="B156" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="14"/>
+      <c r="A157" s="20"/>
       <c r="B157" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="20"/>
       <c r="B158" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="20"/>
       <c r="B159" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="20"/>
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="20"/>
       <c r="B161" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="20"/>
       <c r="B162" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="14"/>
+      <c r="A163" s="20"/>
       <c r="B163" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="14"/>
+      <c r="A164" s="20"/>
       <c r="B164" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="14"/>
+      <c r="A165" s="20"/>
       <c r="B165" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="14"/>
+      <c r="A166" s="20"/>
       <c r="B166" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="14"/>
+      <c r="A167" s="20"/>
       <c r="B167" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="14"/>
+      <c r="A168" s="20"/>
       <c r="B168" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="20"/>
       <c r="B169" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="14"/>
+      <c r="A170" s="20"/>
       <c r="B170" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="20"/>
       <c r="B171" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="20"/>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="14"/>
+      <c r="A173" s="20"/>
       <c r="B173" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="20"/>
       <c r="B174" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="20"/>
       <c r="B175" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="14"/>
+      <c r="A176" s="20"/>
       <c r="B176" s="5"/>
     </row>
     <row r="177" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="14"/>
+      <c r="A177" s="20"/>
       <c r="B177" s="12" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="20"/>
       <c r="B178" s="5"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
+      <c r="A179" s="20"/>
       <c r="B179" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="20"/>
       <c r="B180" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="20"/>
       <c r="B181" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="14"/>
+      <c r="A182" s="20"/>
       <c r="B182" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="20"/>
       <c r="B183" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="14"/>
+      <c r="A184" s="20"/>
       <c r="B184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="20"/>
       <c r="B185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="20"/>
       <c r="B186" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="20"/>
       <c r="B187" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="20"/>
       <c r="B188" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="20"/>
       <c r="B189" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="20"/>
       <c r="B190" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="14"/>
+      <c r="A191" s="20"/>
       <c r="B191" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="20"/>
       <c r="B192" s="5"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="20"/>
       <c r="B193" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="20"/>
       <c r="B194" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="14"/>
+      <c r="A195" s="20"/>
       <c r="B195" s="5"/>
     </row>
     <row r="196" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="14"/>
+      <c r="A196" s="20"/>
       <c r="B196" s="12" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
-      <c r="B197" s="20"/>
+      <c r="A197" s="20"/>
+      <c r="B197" s="16"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
-      <c r="B198" s="19" t="s">
+      <c r="A198" s="20"/>
+      <c r="B198" s="15" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="20"/>
       <c r="B199" s="7"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
-      <c r="B200" s="19" t="s">
+      <c r="A200" s="20"/>
+      <c r="B200" s="15" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="14"/>
+      <c r="A201" s="20"/>
       <c r="B201" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="20"/>
       <c r="B202" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="20"/>
       <c r="B203" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="20"/>
       <c r="B204" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
-      <c r="B205" s="21" t="s">
+      <c r="A205" s="20"/>
+      <c r="B205" s="17" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="20"/>
       <c r="B206" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="14"/>
+      <c r="A207" s="20"/>
       <c r="B207" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="20"/>
       <c r="B208" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="20"/>
       <c r="B209" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
-      <c r="B210" s="19" t="s">
+      <c r="A210" s="20"/>
+      <c r="B210" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="20"/>
       <c r="B211" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="20"/>
       <c r="B212" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="20"/>
       <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
-      <c r="B214" s="19" t="s">
+      <c r="A214" s="20"/>
+      <c r="B214" s="15" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="14"/>
+      <c r="A215" s="20"/>
       <c r="B215" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="20"/>
       <c r="B216" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="20"/>
       <c r="B217" s="3" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="20"/>
       <c r="B218" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="20"/>
       <c r="B219" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="20"/>
       <c r="B220" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="14"/>
+      <c r="A221" s="20"/>
       <c r="B221" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="14"/>
+      <c r="A222" s="20"/>
       <c r="B222" s="7"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="14"/>
-      <c r="B223" s="19" t="s">
+      <c r="A223" s="20"/>
+      <c r="B223" s="15" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="14"/>
+      <c r="A224" s="20"/>
       <c r="B224" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="14"/>
+      <c r="A225" s="20"/>
       <c r="B225" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="14"/>
+      <c r="A226" s="20"/>
       <c r="B226" s="5"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="20"/>
       <c r="B227" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="14"/>
+      <c r="A228" s="20"/>
       <c r="B228" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="14"/>
+      <c r="A229" s="20"/>
       <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="14"/>
+      <c r="A230" s="20"/>
       <c r="B230" s="12" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="14"/>
+      <c r="A231" s="20"/>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
-      <c r="B232" s="19" t="s">
+      <c r="A232" s="20"/>
+      <c r="B232" s="15" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="20"/>
       <c r="B233" s="7"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
-      <c r="B234" s="19" t="s">
+      <c r="A234" s="20"/>
+      <c r="B234" s="15" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="20"/>
       <c r="B235" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="20"/>
       <c r="B236" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="14"/>
+      <c r="A237" s="20"/>
       <c r="B237" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="20"/>
       <c r="B238" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="20"/>
       <c r="B239" s="7"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="14"/>
-      <c r="B240" s="19" t="s">
+      <c r="A240" s="20"/>
+      <c r="B240" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="20"/>
       <c r="B241" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="14"/>
+      <c r="A242" s="20"/>
       <c r="B242" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="20"/>
       <c r="B243" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="20"/>
       <c r="B244" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="20"/>
       <c r="B245" s="7"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
-      <c r="B246" s="19" t="s">
+      <c r="A246" s="20"/>
+      <c r="B246" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="20"/>
       <c r="B247" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="20"/>
       <c r="B248" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="14"/>
+      <c r="A249" s="20"/>
       <c r="B249" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="20"/>
       <c r="B250" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="20"/>
       <c r="B251" s="7"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
-      <c r="B252" s="19" t="s">
+      <c r="A252" s="20"/>
+      <c r="B252" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="20"/>
       <c r="B253" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="20"/>
       <c r="B254" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="20"/>
       <c r="B255" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="20"/>
       <c r="B256" s="7"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
-      <c r="B257" s="19" t="s">
+      <c r="A257" s="20"/>
+      <c r="B257" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="20"/>
       <c r="B258" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="14"/>
+      <c r="A259" s="20"/>
       <c r="B259" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="20"/>
       <c r="B260" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="20"/>
       <c r="B261" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="20"/>
       <c r="B262" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="20"/>
       <c r="B263" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="20"/>
       <c r="B264" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="14"/>
+      <c r="A265" s="20"/>
       <c r="B265" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="20"/>
       <c r="B266" s="7"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
-      <c r="B267" s="19" t="s">
+      <c r="A267" s="20"/>
+      <c r="B267" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="20"/>
       <c r="B268" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="20"/>
       <c r="B269" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="20"/>
       <c r="B270" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="20"/>
       <c r="B271" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="20"/>
       <c r="B272" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="14"/>
+      <c r="A273" s="20"/>
       <c r="B273" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="20"/>
       <c r="B274" s="7"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
-      <c r="B275" s="19" t="s">
+      <c r="A275" s="20"/>
+      <c r="B275" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="20"/>
       <c r="B276" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="20"/>
       <c r="B277" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="20"/>
       <c r="B278" s="7"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="14"/>
-      <c r="B279" s="19" t="s">
+      <c r="A279" s="20"/>
+      <c r="B279" s="15" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="14"/>
+      <c r="A280" s="20"/>
       <c r="B280" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="14"/>
+      <c r="A281" s="20"/>
       <c r="B281" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="14"/>
+      <c r="A282" s="20"/>
       <c r="B282" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="14"/>
+      <c r="A283" s="20"/>
       <c r="B283" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="14"/>
+      <c r="A284" s="20"/>
       <c r="B284" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="20"/>
       <c r="B285" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="14"/>
+      <c r="A286" s="20"/>
       <c r="B286" s="7"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
-      <c r="B287" s="19" t="s">
+      <c r="A287" s="20"/>
+      <c r="B287" s="15" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="20"/>
       <c r="B288" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="14"/>
+      <c r="A289" s="20"/>
       <c r="B289" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="20"/>
       <c r="B290" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="20"/>
       <c r="B291" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="20"/>
       <c r="B292" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="20"/>
       <c r="B293" s="5"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="20"/>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="14"/>
+      <c r="A295" s="20"/>
       <c r="B295" s="5"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="20"/>
       <c r="B296" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="20"/>
       <c r="B297" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="14"/>
+      <c r="A298" s="20"/>
       <c r="B298" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="20"/>
       <c r="B299" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="14"/>
+      <c r="A300" s="20"/>
       <c r="B300" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="20"/>
       <c r="B301" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="20"/>
       <c r="B302" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="20"/>
       <c r="B303" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="20"/>
       <c r="B304" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="20"/>
       <c r="B305" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="20"/>
       <c r="B306" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="20"/>
       <c r="B307" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="14"/>
+      <c r="A308" s="20"/>
       <c r="B308" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="20"/>
       <c r="B309" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="20"/>
       <c r="B310" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="20"/>
       <c r="B311" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="15"/>
+      <c r="A312" s="22"/>
       <c r="B312" s="9"/>
     </row>
     <row r="315" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="316" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A316" s="16" t="s">
+      <c r="A316" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B316" s="17" t="s">
-        <v>3</v>
+      <c r="B316" s="14" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="20"/>
       <c r="B317" s="1"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="14"/>
+      <c r="A318" s="20"/>
       <c r="B318" s="3"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="20"/>
       <c r="B319" s="2"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="20"/>
       <c r="B320" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="20"/>
       <c r="B321" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="20"/>
       <c r="B322" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="20"/>
       <c r="B323" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="20"/>
       <c r="B324" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="14"/>
+      <c r="A325" s="20"/>
       <c r="B325" s="10" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="20"/>
       <c r="B326" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="18"/>
+      <c r="A327" s="21"/>
       <c r="B327" s="10" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="20"/>
       <c r="B328" s="10" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="20"/>
       <c r="B329" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="20"/>
       <c r="B330" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="20"/>
       <c r="B331" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="20"/>
       <c r="B332" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="14"/>
+      <c r="A333" s="20"/>
       <c r="B333" s="10" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="20"/>
       <c r="B334" s="10" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="20"/>
       <c r="B335" s="10" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="20"/>
       <c r="B336" s="10" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="20"/>
       <c r="B337" s="10" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="20"/>
       <c r="B338" s="10" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="14"/>
+      <c r="A339" s="20"/>
       <c r="B339" s="10" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="14"/>
+      <c r="A340" s="20"/>
       <c r="B340" s="10" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="14"/>
+      <c r="A341" s="20"/>
       <c r="B341" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="14"/>
+      <c r="A342" s="20"/>
       <c r="B342" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="14"/>
+      <c r="A343" s="20"/>
       <c r="B343" s="3"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="14"/>
+      <c r="A344" s="20"/>
       <c r="B344" s="7"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="20"/>
       <c r="B345" s="3"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="14"/>
+      <c r="A346" s="20"/>
       <c r="B346" s="3"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="20"/>
       <c r="B347" s="5" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="20"/>
       <c r="B348" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="14"/>
+      <c r="A349" s="20"/>
       <c r="B349" s="6" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="20"/>
       <c r="B350" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
-      <c r="B351" s="22" t="s">
+      <c r="A351" s="20"/>
+      <c r="B351" s="18" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
-      <c r="B352" s="22" t="s">
+      <c r="A352" s="20"/>
+      <c r="B352" s="18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+    <row r="353" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A353" s="20"/>
       <c r="B353" s="5"/>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="18"/>
-      <c r="B354" s="3"/>
+    <row r="354" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="21"/>
+      <c r="B354" s="14" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="14"/>
+      <c r="A355" s="20"/>
       <c r="B355" s="5"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
-      <c r="B356" s="3"/>
+      <c r="A356" s="20"/>
+      <c r="B356" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
-      <c r="B357" s="3"/>
+      <c r="A357" s="20"/>
+      <c r="B357" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="14"/>
-      <c r="B358" s="8"/>
+      <c r="A358" s="20"/>
+      <c r="B358" s="8" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
-      <c r="B359" s="7"/>
+      <c r="A359" s="20"/>
+      <c r="B359" s="23" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="14"/>
-      <c r="B360" s="3"/>
+      <c r="A360" s="20"/>
+      <c r="B360" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
-      <c r="B361" s="7"/>
+      <c r="A361" s="20"/>
+      <c r="B361" s="23" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
-      <c r="B362" s="8"/>
+      <c r="A362" s="20"/>
+      <c r="B362" s="11" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="20"/>
       <c r="B363" s="3"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="20"/>
       <c r="B364" s="5"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="20"/>
       <c r="B365" s="5"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
-      <c r="B366" s="5"/>
+      <c r="A366" s="20"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
-      <c r="B367" s="5"/>
+      <c r="A367" s="20"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="14"/>
+      <c r="A368" s="20"/>
       <c r="B368" s="5"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="18"/>
+      <c r="A369" s="21"/>
       <c r="B369" s="3"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="20"/>
       <c r="B370" s="5"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="20"/>
       <c r="B371" s="3"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="20"/>
       <c r="B372" s="8"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="20"/>
       <c r="B373" s="7"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="20"/>
       <c r="B374" s="3"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="20"/>
       <c r="B375" s="3"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="20"/>
       <c r="B376" s="3"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="20"/>
       <c r="B377" s="3"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="14"/>
+      <c r="A378" s="20"/>
       <c r="B378" s="3"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="20"/>
       <c r="B379" s="3"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="20"/>
       <c r="B380" s="3"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="20"/>
       <c r="B381" s="3"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="20"/>
       <c r="B382" s="3"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="20"/>
       <c r="B383" s="3"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="20"/>
       <c r="B384" s="3"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="14"/>
+      <c r="A385" s="20"/>
       <c r="B385" s="7"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="20"/>
       <c r="B386" s="8"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="20"/>
       <c r="B387" s="7"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="20"/>
       <c r="B388" s="3"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="20"/>
       <c r="B389" s="3"/>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="20"/>
       <c r="B390" s="3"/>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="20"/>
       <c r="B391" s="7"/>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="20"/>
       <c r="B392" s="8"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="14"/>
+      <c r="A393" s="20"/>
       <c r="B393" s="3"/>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="20"/>
       <c r="B394" s="5"/>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="20"/>
       <c r="B395" s="5"/>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="20"/>
       <c r="B396" s="5"/>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="20"/>
       <c r="B397" s="3"/>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="18"/>
+      <c r="A398" s="21"/>
       <c r="B398" s="3"/>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="14"/>
+      <c r="A399" s="20"/>
       <c r="B399" s="3"/>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="14"/>
+      <c r="A400" s="20"/>
       <c r="B400" s="8"/>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="14"/>
+      <c r="A401" s="20"/>
       <c r="B401" s="5"/>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="14"/>
+      <c r="A402" s="20"/>
       <c r="B402" s="11"/>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="14"/>
+      <c r="A403" s="20"/>
       <c r="B403" s="3"/>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="18"/>
+      <c r="A404" s="21"/>
       <c r="B404" s="3"/>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="20"/>
       <c r="B405" s="3"/>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="14"/>
+      <c r="A406" s="20"/>
       <c r="B406" s="3"/>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="20"/>
       <c r="B407" s="3"/>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="20"/>
       <c r="B408" s="5"/>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="14"/>
+      <c r="A409" s="20"/>
       <c r="B409" s="5"/>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="20"/>
       <c r="B410" s="3"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="18"/>
+      <c r="A411" s="21"/>
       <c r="B411" s="3"/>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="20"/>
       <c r="B412" s="3"/>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="20"/>
       <c r="B413" s="3"/>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="20"/>
       <c r="B414" s="3"/>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="14"/>
+      <c r="A415" s="20"/>
       <c r="B415" s="3"/>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="20"/>
       <c r="B416" s="3"/>
     </row>
     <row r="417" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A417" s="15"/>
+      <c r="A417" s="22"/>
       <c r="B417" s="9"/>
     </row>
   </sheetData>
@@ -14050,5 +14588,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizado o form002 e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BFB793-A488-4CC0-95A8-C8D423F4A35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8018F04-B29D-46B5-B879-2674BDF32BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="246">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -11645,6 +11645,1421 @@
         <family val="3"/>
       </rPr>
       <t>. E os dois têm a mesma performance.</t>
+    </r>
+  </si>
+  <si>
+    <t>Aula 4 – Atributos para input text e password</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Document&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Teste de formulário&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"container"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iusu"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Usuário: &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"isen"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Senha: &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Enviar"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"reset"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Limpar"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>O input tipo text é para digitar texto como usuário. O input tipo password é para digitar senha (oculta o que foi digitado). Submit é botão de enviar e reset é botão para limpar.</t>
+  </si>
+  <si>
+    <t>O required dentro dos inputs serve para dar uma mensagem de erro caso o usuário tente enviar o formulário sem preencher os campos com esse atributo.</t>
+  </si>
+  <si>
+    <t>O minlength serve para definir o mínimo de caracteres para cada input, o maxlength serve para definir o máximo de caracteres. O próprio navegador faz a validação em js...</t>
+  </si>
+  <si>
+    <t>O size serve para ajustar o tamanho da caixa, mesmo que tenha configurado um size de 8, ele vai caber quantas caracteres difinir no maxlength, vai ter uma rolagem lateral...</t>
+  </si>
+  <si>
+    <t>O placeholder serve para colocar alguma informação dentro da caixa. Ex.: Na caixa da label Usuário colocar um placeholder com "nome do usuário"</t>
+  </si>
+  <si>
+    <t>O auto complete on no form habilita colocar o auto complete nos inputs também, no caso do primeiro coloca o username e o da senha current-password, e tem o new-password também.</t>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"post"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"cadastro.php"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"post"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"on"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"usu"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iusu"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>minlength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>maxlength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"30"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"15"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>placeholder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Nome do Usuário"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"username"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"sen"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"isen"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>minlength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"6"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"15"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>placeholder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Senha de 6 dígitos"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"current-password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
     </r>
   </si>
 </sst>
@@ -11831,7 +13246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -11924,11 +13339,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -11951,9 +13397,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -11973,9 +13416,6 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -11988,9 +13428,36 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12354,16 +13821,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B417"/>
+  <dimension ref="A2:B456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView tabSelected="1" topLeftCell="B389" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B399" sqref="B399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="211.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="225" style="4" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -12377,2214 +13844,2442 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="14" t="s">
+      <c r="A42" s="19"/>
+      <c r="B42" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="20"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="14" t="s">
+      <c r="A57" s="19"/>
+      <c r="B57" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="7"/>
     </row>
     <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="20"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="7"/>
     </row>
     <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
+      <c r="A80" s="18"/>
       <c r="B80" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
+      <c r="A81" s="18"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="18"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
+      <c r="A84" s="18"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
+      <c r="A85" s="18"/>
       <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="21"/>
-      <c r="B86" s="14" t="s">
+      <c r="A86" s="19"/>
+      <c r="B86" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
+      <c r="A87" s="18"/>
       <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
+      <c r="A88" s="18"/>
       <c r="B88" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
+      <c r="A89" s="18"/>
       <c r="B89" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
-      <c r="B90" s="11" t="s">
+      <c r="A90" s="18"/>
+      <c r="B90" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="20"/>
+      <c r="A91" s="18"/>
       <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="21"/>
-      <c r="B92" s="14" t="s">
+      <c r="A92" s="19"/>
+      <c r="B92" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
+      <c r="A93" s="18"/>
       <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="20"/>
+      <c r="A94" s="18"/>
       <c r="B94" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="20"/>
+      <c r="A95" s="18"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="20"/>
+      <c r="A96" s="18"/>
       <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="20"/>
+      <c r="A97" s="18"/>
       <c r="B97" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="20"/>
+      <c r="A98" s="18"/>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="21"/>
-      <c r="B99" s="14" t="s">
+      <c r="A99" s="19"/>
+      <c r="B99" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="20"/>
+      <c r="A100" s="18"/>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="20"/>
+      <c r="A101" s="18"/>
       <c r="B101" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="20"/>
+      <c r="A102" s="18"/>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="20"/>
+      <c r="A103" s="18"/>
       <c r="B103" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="20"/>
+      <c r="A104" s="18"/>
       <c r="B104" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="22"/>
+      <c r="A105" s="20"/>
       <c r="B105" s="9"/>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="19" t="s">
+      <c r="A109" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="20"/>
-      <c r="B110" s="12" t="s">
+      <c r="A110" s="18"/>
+      <c r="B110" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="20"/>
+      <c r="A111" s="18"/>
       <c r="B111" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="20"/>
+      <c r="A112" s="18"/>
       <c r="B112" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="20"/>
+      <c r="A113" s="18"/>
       <c r="B113" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
+      <c r="A114" s="18"/>
       <c r="B114" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
+      <c r="A115" s="18"/>
       <c r="B115" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
+      <c r="A116" s="18"/>
       <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="20"/>
+      <c r="A117" s="18"/>
       <c r="B117" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="20"/>
+      <c r="A118" s="18"/>
       <c r="B118" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="20"/>
+      <c r="A119" s="18"/>
       <c r="B119" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="20"/>
+      <c r="A120" s="18"/>
       <c r="B120" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="20"/>
+      <c r="A121" s="18"/>
       <c r="B121" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="20"/>
+      <c r="A122" s="18"/>
       <c r="B122" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="20"/>
+      <c r="A123" s="18"/>
       <c r="B123" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="20"/>
+      <c r="A124" s="18"/>
       <c r="B124" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="20"/>
+      <c r="A125" s="18"/>
       <c r="B125" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="20"/>
+      <c r="A126" s="18"/>
       <c r="B126" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="20"/>
+      <c r="A127" s="18"/>
       <c r="B127" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="20"/>
+      <c r="A128" s="18"/>
       <c r="B128" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="20"/>
+      <c r="A129" s="18"/>
       <c r="B129" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="20"/>
+      <c r="A130" s="18"/>
       <c r="B130" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="20"/>
+      <c r="A131" s="18"/>
       <c r="B131" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="20"/>
+      <c r="A132" s="18"/>
       <c r="B132" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="20"/>
+      <c r="A133" s="18"/>
       <c r="B133" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="20"/>
+      <c r="A134" s="18"/>
       <c r="B134" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="20"/>
+      <c r="A135" s="18"/>
       <c r="B135" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="20"/>
+      <c r="A136" s="18"/>
       <c r="B136" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="20"/>
+      <c r="A137" s="18"/>
       <c r="B137" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="20"/>
+      <c r="A138" s="18"/>
       <c r="B138" s="3"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="20"/>
+      <c r="A139" s="18"/>
       <c r="B139" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="20"/>
+      <c r="A140" s="18"/>
       <c r="B140" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="20"/>
+      <c r="A141" s="18"/>
       <c r="B141" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="20"/>
-      <c r="B142" s="13" t="s">
+      <c r="A142" s="18"/>
+      <c r="B142" s="12" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="20"/>
-      <c r="B143" s="13" t="s">
+      <c r="A143" s="18"/>
+      <c r="B143" s="12" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="20"/>
-      <c r="B144" s="13" t="s">
+      <c r="A144" s="18"/>
+      <c r="B144" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="20"/>
+      <c r="A145" s="18"/>
       <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="20"/>
-      <c r="B146" s="12" t="s">
+      <c r="A146" s="18"/>
+      <c r="B146" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="20"/>
+      <c r="A147" s="18"/>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="20"/>
+      <c r="A148" s="18"/>
       <c r="B148" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="20"/>
+      <c r="A149" s="18"/>
       <c r="B149" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="20"/>
+      <c r="A150" s="18"/>
       <c r="B150" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="20"/>
+      <c r="A151" s="18"/>
       <c r="B151" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="20"/>
+      <c r="A152" s="18"/>
       <c r="B152" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="20"/>
+      <c r="A153" s="18"/>
       <c r="B153" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="20"/>
+      <c r="A154" s="18"/>
       <c r="B154" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="20"/>
+      <c r="A155" s="18"/>
       <c r="B155" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="20"/>
+      <c r="A156" s="18"/>
       <c r="B156" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="20"/>
+      <c r="A157" s="18"/>
       <c r="B157" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="20"/>
+      <c r="A158" s="18"/>
       <c r="B158" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="20"/>
+      <c r="A159" s="18"/>
       <c r="B159" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="20"/>
+      <c r="A160" s="18"/>
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="20"/>
+      <c r="A161" s="18"/>
       <c r="B161" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
+      <c r="A162" s="18"/>
       <c r="B162" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
+      <c r="A163" s="18"/>
       <c r="B163" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="20"/>
+      <c r="A164" s="18"/>
       <c r="B164" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="20"/>
+      <c r="A165" s="18"/>
       <c r="B165" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="20"/>
+      <c r="A166" s="18"/>
       <c r="B166" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="20"/>
+      <c r="A167" s="18"/>
       <c r="B167" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="20"/>
+      <c r="A168" s="18"/>
       <c r="B168" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="20"/>
+      <c r="A169" s="18"/>
       <c r="B169" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="20"/>
+      <c r="A170" s="18"/>
       <c r="B170" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="20"/>
+      <c r="A171" s="18"/>
       <c r="B171" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="20"/>
+      <c r="A172" s="18"/>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="20"/>
+      <c r="A173" s="18"/>
       <c r="B173" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="20"/>
+      <c r="A174" s="18"/>
       <c r="B174" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="20"/>
+      <c r="A175" s="18"/>
       <c r="B175" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="20"/>
+      <c r="A176" s="18"/>
       <c r="B176" s="5"/>
     </row>
     <row r="177" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="20"/>
-      <c r="B177" s="12" t="s">
+      <c r="A177" s="18"/>
+      <c r="B177" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="20"/>
+      <c r="A178" s="18"/>
       <c r="B178" s="5"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="20"/>
+      <c r="A179" s="18"/>
       <c r="B179" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="20"/>
+      <c r="A180" s="18"/>
       <c r="B180" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="20"/>
+      <c r="A181" s="18"/>
       <c r="B181" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="20"/>
+      <c r="A182" s="18"/>
       <c r="B182" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="20"/>
+      <c r="A183" s="18"/>
       <c r="B183" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="20"/>
+      <c r="A184" s="18"/>
       <c r="B184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="20"/>
+      <c r="A185" s="18"/>
       <c r="B185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="20"/>
+      <c r="A186" s="18"/>
       <c r="B186" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="20"/>
+      <c r="A187" s="18"/>
       <c r="B187" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="20"/>
+      <c r="A188" s="18"/>
       <c r="B188" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="20"/>
+      <c r="A189" s="18"/>
       <c r="B189" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="20"/>
+      <c r="A190" s="18"/>
       <c r="B190" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="20"/>
+      <c r="A191" s="18"/>
       <c r="B191" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="20"/>
+      <c r="A192" s="18"/>
       <c r="B192" s="5"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="20"/>
+      <c r="A193" s="18"/>
       <c r="B193" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="20"/>
+      <c r="A194" s="18"/>
       <c r="B194" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="20"/>
+      <c r="A195" s="18"/>
       <c r="B195" s="5"/>
     </row>
     <row r="196" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="20"/>
-      <c r="B196" s="12" t="s">
+      <c r="A196" s="18"/>
+      <c r="B196" s="11" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="20"/>
-      <c r="B197" s="16"/>
+      <c r="A197" s="18"/>
+      <c r="B197" s="15"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="20"/>
-      <c r="B198" s="15" t="s">
+      <c r="A198" s="18"/>
+      <c r="B198" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="20"/>
+      <c r="A199" s="18"/>
       <c r="B199" s="7"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="20"/>
-      <c r="B200" s="15" t="s">
+      <c r="A200" s="18"/>
+      <c r="B200" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="20"/>
+      <c r="A201" s="18"/>
       <c r="B201" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="20"/>
+      <c r="A202" s="18"/>
       <c r="B202" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="20"/>
+      <c r="A203" s="18"/>
       <c r="B203" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="20"/>
+      <c r="A204" s="18"/>
       <c r="B204" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="20"/>
-      <c r="B205" s="17" t="s">
+      <c r="A205" s="18"/>
+      <c r="B205" s="16" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="20"/>
+      <c r="A206" s="18"/>
       <c r="B206" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="20"/>
+      <c r="A207" s="18"/>
       <c r="B207" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="20"/>
+      <c r="A208" s="18"/>
       <c r="B208" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="20"/>
+      <c r="A209" s="18"/>
       <c r="B209" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="20"/>
-      <c r="B210" s="15" t="s">
+      <c r="A210" s="18"/>
+      <c r="B210" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="20"/>
+      <c r="A211" s="18"/>
       <c r="B211" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="20"/>
+      <c r="A212" s="18"/>
       <c r="B212" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="20"/>
+      <c r="A213" s="18"/>
       <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="20"/>
-      <c r="B214" s="15" t="s">
+      <c r="A214" s="18"/>
+      <c r="B214" s="14" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="20"/>
+      <c r="A215" s="18"/>
       <c r="B215" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="20"/>
+      <c r="A216" s="18"/>
       <c r="B216" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="20"/>
+      <c r="A217" s="18"/>
       <c r="B217" s="3" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="20"/>
+      <c r="A218" s="18"/>
       <c r="B218" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="20"/>
+      <c r="A219" s="18"/>
       <c r="B219" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="20"/>
+      <c r="A220" s="18"/>
       <c r="B220" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="20"/>
+      <c r="A221" s="18"/>
       <c r="B221" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="20"/>
+      <c r="A222" s="18"/>
       <c r="B222" s="7"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="20"/>
-      <c r="B223" s="15" t="s">
+      <c r="A223" s="18"/>
+      <c r="B223" s="14" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="20"/>
+      <c r="A224" s="18"/>
       <c r="B224" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="20"/>
+      <c r="A225" s="18"/>
       <c r="B225" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="20"/>
+      <c r="A226" s="18"/>
       <c r="B226" s="5"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="20"/>
+      <c r="A227" s="18"/>
       <c r="B227" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="20"/>
+      <c r="A228" s="18"/>
       <c r="B228" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="20"/>
+      <c r="A229" s="18"/>
       <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="20"/>
-      <c r="B230" s="12" t="s">
+      <c r="A230" s="18"/>
+      <c r="B230" s="11" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="20"/>
+      <c r="A231" s="18"/>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="20"/>
-      <c r="B232" s="15" t="s">
+      <c r="A232" s="18"/>
+      <c r="B232" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="20"/>
+      <c r="A233" s="18"/>
       <c r="B233" s="7"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="20"/>
-      <c r="B234" s="15" t="s">
+      <c r="A234" s="18"/>
+      <c r="B234" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="20"/>
+      <c r="A235" s="18"/>
       <c r="B235" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="20"/>
+      <c r="A236" s="18"/>
       <c r="B236" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="20"/>
+      <c r="A237" s="18"/>
       <c r="B237" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="20"/>
+      <c r="A238" s="18"/>
       <c r="B238" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="20"/>
+      <c r="A239" s="18"/>
       <c r="B239" s="7"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="20"/>
-      <c r="B240" s="15" t="s">
+      <c r="A240" s="18"/>
+      <c r="B240" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="20"/>
+      <c r="A241" s="18"/>
       <c r="B241" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="20"/>
+      <c r="A242" s="18"/>
       <c r="B242" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="20"/>
+      <c r="A243" s="18"/>
       <c r="B243" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="20"/>
+      <c r="A244" s="18"/>
       <c r="B244" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="20"/>
+      <c r="A245" s="18"/>
       <c r="B245" s="7"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="20"/>
-      <c r="B246" s="15" t="s">
+      <c r="A246" s="18"/>
+      <c r="B246" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="20"/>
+      <c r="A247" s="18"/>
       <c r="B247" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="20"/>
+      <c r="A248" s="18"/>
       <c r="B248" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="20"/>
+      <c r="A249" s="18"/>
       <c r="B249" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="20"/>
+      <c r="A250" s="18"/>
       <c r="B250" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="20"/>
+      <c r="A251" s="18"/>
       <c r="B251" s="7"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="20"/>
-      <c r="B252" s="15" t="s">
+      <c r="A252" s="18"/>
+      <c r="B252" s="14" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="20"/>
+      <c r="A253" s="18"/>
       <c r="B253" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="20"/>
+      <c r="A254" s="18"/>
       <c r="B254" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="20"/>
+      <c r="A255" s="18"/>
       <c r="B255" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="20"/>
+      <c r="A256" s="18"/>
       <c r="B256" s="7"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="20"/>
-      <c r="B257" s="15" t="s">
+      <c r="A257" s="18"/>
+      <c r="B257" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="20"/>
+      <c r="A258" s="18"/>
       <c r="B258" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="20"/>
+      <c r="A259" s="18"/>
       <c r="B259" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="20"/>
+      <c r="A260" s="18"/>
       <c r="B260" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="20"/>
+      <c r="A261" s="18"/>
       <c r="B261" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="20"/>
+      <c r="A262" s="18"/>
       <c r="B262" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="20"/>
+      <c r="A263" s="18"/>
       <c r="B263" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="20"/>
+      <c r="A264" s="18"/>
       <c r="B264" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="20"/>
+      <c r="A265" s="18"/>
       <c r="B265" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="20"/>
+      <c r="A266" s="18"/>
       <c r="B266" s="7"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="20"/>
-      <c r="B267" s="15" t="s">
+      <c r="A267" s="18"/>
+      <c r="B267" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="20"/>
+      <c r="A268" s="18"/>
       <c r="B268" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="20"/>
+      <c r="A269" s="18"/>
       <c r="B269" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="20"/>
+      <c r="A270" s="18"/>
       <c r="B270" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="20"/>
+      <c r="A271" s="18"/>
       <c r="B271" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="20"/>
+      <c r="A272" s="18"/>
       <c r="B272" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="20"/>
+      <c r="A273" s="18"/>
       <c r="B273" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="20"/>
+      <c r="A274" s="18"/>
       <c r="B274" s="7"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="20"/>
-      <c r="B275" s="15" t="s">
+      <c r="A275" s="18"/>
+      <c r="B275" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="20"/>
+      <c r="A276" s="18"/>
       <c r="B276" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="20"/>
+      <c r="A277" s="18"/>
       <c r="B277" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="20"/>
+      <c r="A278" s="18"/>
       <c r="B278" s="7"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="20"/>
-      <c r="B279" s="15" t="s">
+      <c r="A279" s="18"/>
+      <c r="B279" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="20"/>
+      <c r="A280" s="18"/>
       <c r="B280" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="20"/>
+      <c r="A281" s="18"/>
       <c r="B281" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="20"/>
+      <c r="A282" s="18"/>
       <c r="B282" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="20"/>
+      <c r="A283" s="18"/>
       <c r="B283" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="20"/>
+      <c r="A284" s="18"/>
       <c r="B284" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="20"/>
+      <c r="A285" s="18"/>
       <c r="B285" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="20"/>
+      <c r="A286" s="18"/>
       <c r="B286" s="7"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="20"/>
-      <c r="B287" s="15" t="s">
+      <c r="A287" s="18"/>
+      <c r="B287" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="20"/>
+      <c r="A288" s="18"/>
       <c r="B288" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="20"/>
+      <c r="A289" s="18"/>
       <c r="B289" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="20"/>
+      <c r="A290" s="18"/>
       <c r="B290" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="20"/>
+      <c r="A291" s="18"/>
       <c r="B291" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="20"/>
+      <c r="A292" s="18"/>
       <c r="B292" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="20"/>
+      <c r="A293" s="18"/>
       <c r="B293" s="5"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="20"/>
+      <c r="A294" s="18"/>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="20"/>
+      <c r="A295" s="18"/>
       <c r="B295" s="5"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="20"/>
+      <c r="A296" s="18"/>
       <c r="B296" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="20"/>
+      <c r="A297" s="18"/>
       <c r="B297" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="20"/>
+      <c r="A298" s="18"/>
       <c r="B298" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="20"/>
+      <c r="A299" s="18"/>
       <c r="B299" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="20"/>
+      <c r="A300" s="18"/>
       <c r="B300" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="20"/>
+      <c r="A301" s="18"/>
       <c r="B301" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="20"/>
+      <c r="A302" s="18"/>
       <c r="B302" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="20"/>
+      <c r="A303" s="18"/>
       <c r="B303" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="20"/>
+      <c r="A304" s="18"/>
       <c r="B304" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="20"/>
+      <c r="A305" s="18"/>
       <c r="B305" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="20"/>
+      <c r="A306" s="18"/>
       <c r="B306" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="20"/>
+      <c r="A307" s="18"/>
       <c r="B307" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="20"/>
+      <c r="A308" s="18"/>
       <c r="B308" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="20"/>
+      <c r="A309" s="18"/>
       <c r="B309" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="20"/>
+      <c r="A310" s="18"/>
       <c r="B310" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="20"/>
+      <c r="A311" s="18"/>
       <c r="B311" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="22"/>
+      <c r="A312" s="20"/>
       <c r="B312" s="9"/>
     </row>
     <row r="315" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="316" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A316" s="19" t="s">
+    <row r="316" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="B316" s="14" t="s">
+      <c r="B316" s="13" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="20"/>
-      <c r="B317" s="1"/>
+      <c r="A317" s="18"/>
+      <c r="B317" s="21"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="20"/>
-      <c r="B318" s="3"/>
+      <c r="A318" s="18"/>
+      <c r="B318" s="22"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="20"/>
-      <c r="B319" s="2"/>
+      <c r="A319" s="18"/>
+      <c r="B319" s="23"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="20"/>
-      <c r="B320" s="10" t="s">
+      <c r="A320" s="18"/>
+      <c r="B320" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="20"/>
-      <c r="B321" s="10" t="s">
+      <c r="A321" s="18"/>
+      <c r="B321" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="20"/>
-      <c r="B322" s="10" t="s">
+      <c r="A322" s="18"/>
+      <c r="B322" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="20"/>
-      <c r="B323" s="10" t="s">
+      <c r="A323" s="18"/>
+      <c r="B323" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="20"/>
-      <c r="B324" s="10" t="s">
+      <c r="A324" s="18"/>
+      <c r="B324" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="20"/>
-      <c r="B325" s="10" t="s">
+      <c r="A325" s="18"/>
+      <c r="B325" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="20"/>
-      <c r="B326" s="10" t="s">
+      <c r="A326" s="18"/>
+      <c r="B326" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="21"/>
-      <c r="B327" s="10" t="s">
+      <c r="A327" s="18"/>
+      <c r="B327" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="20"/>
-      <c r="B328" s="10" t="s">
+      <c r="A328" s="18"/>
+      <c r="B328" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="20"/>
-      <c r="B329" s="10" t="s">
+      <c r="A329" s="18"/>
+      <c r="B329" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="20"/>
-      <c r="B330" s="10" t="s">
+      <c r="A330" s="18"/>
+      <c r="B330" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="20"/>
-      <c r="B331" s="10" t="s">
+      <c r="A331" s="18"/>
+      <c r="B331" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="20"/>
-      <c r="B332" s="10" t="s">
+      <c r="A332" s="18"/>
+      <c r="B332" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="20"/>
-      <c r="B333" s="10" t="s">
+      <c r="A333" s="18"/>
+      <c r="B333" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="20"/>
-      <c r="B334" s="10" t="s">
+      <c r="A334" s="18"/>
+      <c r="B334" s="3" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="20"/>
-      <c r="B335" s="10" t="s">
+      <c r="A335" s="18"/>
+      <c r="B335" s="3" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="20"/>
-      <c r="B336" s="10" t="s">
+      <c r="A336" s="18"/>
+      <c r="B336" s="3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="20"/>
-      <c r="B337" s="10" t="s">
+      <c r="A337" s="18"/>
+      <c r="B337" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="20"/>
-      <c r="B338" s="10" t="s">
+      <c r="A338" s="18"/>
+      <c r="B338" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="20"/>
-      <c r="B339" s="10" t="s">
+      <c r="A339" s="18"/>
+      <c r="B339" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="20"/>
-      <c r="B340" s="10" t="s">
+      <c r="A340" s="18"/>
+      <c r="B340" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="20"/>
-      <c r="B341" s="10" t="s">
+      <c r="A341" s="18"/>
+      <c r="B341" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="20"/>
-      <c r="B342" s="10" t="s">
+      <c r="A342" s="18"/>
+      <c r="B342" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="20"/>
+      <c r="A343" s="18"/>
       <c r="B343" s="3"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="20"/>
-      <c r="B344" s="7"/>
+      <c r="A344" s="18"/>
+      <c r="B344" s="24"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="20"/>
-      <c r="B345" s="3"/>
+      <c r="A345" s="18"/>
+      <c r="B345" s="22"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="20"/>
-      <c r="B346" s="3"/>
+      <c r="A346" s="18"/>
+      <c r="B346" s="22"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="20"/>
-      <c r="B347" s="5" t="s">
+      <c r="A347" s="18"/>
+      <c r="B347" s="25" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" s="20"/>
-      <c r="B348" s="5" t="s">
+      <c r="A348" s="18"/>
+      <c r="B348" s="25" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="20"/>
-      <c r="B349" s="6" t="s">
+      <c r="A349" s="18"/>
+      <c r="B349" s="26" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" s="20"/>
-      <c r="B350" s="5" t="s">
+      <c r="A350" s="18"/>
+      <c r="B350" s="25" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" s="20"/>
-      <c r="B351" s="18" t="s">
+      <c r="A351" s="18"/>
+      <c r="B351" s="27" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" s="20"/>
-      <c r="B352" s="18" t="s">
+      <c r="A352" s="18"/>
+      <c r="B352" s="27" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A353" s="20"/>
-      <c r="B353" s="5"/>
+      <c r="A353" s="18"/>
+      <c r="B353" s="25"/>
     </row>
     <row r="354" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A354" s="21"/>
-      <c r="B354" s="14" t="s">
+      <c r="A354" s="19"/>
+      <c r="B354" s="13" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="20"/>
-      <c r="B355" s="5"/>
+      <c r="A355" s="18"/>
+      <c r="B355" s="25"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" s="20"/>
-      <c r="B356" s="5" t="s">
+      <c r="A356" s="18"/>
+      <c r="B356" s="25" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" s="20"/>
-      <c r="B357" s="5" t="s">
+      <c r="A357" s="18"/>
+      <c r="B357" s="25" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="20"/>
-      <c r="B358" s="8" t="s">
+      <c r="A358" s="18"/>
+      <c r="B358" s="28" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="20"/>
-      <c r="B359" s="23" t="s">
+      <c r="A359" s="18"/>
+      <c r="B359" s="29" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="20"/>
-      <c r="B360" s="3" t="s">
+      <c r="A360" s="18"/>
+      <c r="B360" s="22" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="20"/>
-      <c r="B361" s="23" t="s">
+      <c r="A361" s="18"/>
+      <c r="B361" s="29" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="20"/>
-      <c r="B362" s="11" t="s">
+      <c r="A362" s="18"/>
+      <c r="B362" s="30" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="20"/>
-      <c r="B363" s="3"/>
+      <c r="A363" s="18"/>
+      <c r="B363" s="22"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="20"/>
-      <c r="B364" s="5"/>
+      <c r="A364" s="18"/>
+      <c r="B364" s="25"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="20"/>
-      <c r="B365" s="5"/>
+      <c r="A365" s="18"/>
+      <c r="B365" s="25"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="20"/>
+      <c r="A366" s="18"/>
+      <c r="B366" s="32"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="20"/>
+      <c r="A367" s="18"/>
+      <c r="B367" s="32"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="20"/>
+      <c r="A368" s="18"/>
       <c r="B368" s="5"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="21"/>
-      <c r="B369" s="3"/>
+      <c r="A369" s="18"/>
+      <c r="B369" s="22"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="20"/>
-      <c r="B370" s="5"/>
+      <c r="A370" s="18"/>
+      <c r="B370" s="25"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="20"/>
-      <c r="B371" s="3"/>
+      <c r="A371" s="18"/>
+      <c r="B371" s="22"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="20"/>
-      <c r="B372" s="8"/>
+      <c r="A372" s="18"/>
+      <c r="B372" s="28"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="20"/>
-      <c r="B373" s="7"/>
+      <c r="A373" s="18"/>
+      <c r="B373" s="24"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="20"/>
-      <c r="B374" s="3"/>
+      <c r="A374" s="18"/>
+      <c r="B374" s="22"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="20"/>
-      <c r="B375" s="3"/>
+      <c r="A375" s="18"/>
+      <c r="B375" s="22"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="20"/>
-      <c r="B376" s="3"/>
+      <c r="A376" s="18"/>
+      <c r="B376" s="22"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="20"/>
-      <c r="B377" s="3"/>
+      <c r="A377" s="18"/>
+      <c r="B377" s="22"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="20"/>
-      <c r="B378" s="3"/>
+      <c r="A378" s="18"/>
+      <c r="B378" s="22"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="20"/>
-      <c r="B379" s="3"/>
+      <c r="A379" s="18"/>
+      <c r="B379" s="22"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="20"/>
-      <c r="B380" s="3"/>
+      <c r="A380" s="18"/>
+      <c r="B380" s="22"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="20"/>
-      <c r="B381" s="3"/>
+      <c r="A381" s="18"/>
+      <c r="B381" s="22"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="20"/>
-      <c r="B382" s="3"/>
+      <c r="A382" s="18"/>
+      <c r="B382" s="22"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="20"/>
-      <c r="B383" s="3"/>
+      <c r="A383" s="18"/>
+      <c r="B383" s="22"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="20"/>
-      <c r="B384" s="3"/>
+      <c r="A384" s="18"/>
+      <c r="B384" s="22"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="20"/>
-      <c r="B385" s="7"/>
+      <c r="A385" s="18"/>
+      <c r="B385" s="24"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="20"/>
-      <c r="B386" s="8"/>
+      <c r="A386" s="18"/>
+      <c r="B386" s="28"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="20"/>
-      <c r="B387" s="7"/>
+      <c r="A387" s="18"/>
+      <c r="B387" s="24"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="20"/>
-      <c r="B388" s="3"/>
+      <c r="A388" s="18"/>
+      <c r="B388" s="22"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="20"/>
-      <c r="B389" s="3"/>
+      <c r="A389" s="18"/>
+      <c r="B389" s="22"/>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="20"/>
-      <c r="B390" s="3"/>
+      <c r="A390" s="18"/>
+      <c r="B390" s="22"/>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="20"/>
-      <c r="B391" s="7"/>
+      <c r="A391" s="18"/>
+      <c r="B391" s="24"/>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="20"/>
-      <c r="B392" s="8"/>
+      <c r="A392" s="18"/>
+      <c r="B392" s="28"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="20"/>
-      <c r="B393" s="3"/>
+      <c r="A393" s="18"/>
+      <c r="B393" s="22"/>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="20"/>
-      <c r="B394" s="5"/>
+      <c r="A394" s="18"/>
+      <c r="B394" s="25"/>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="20"/>
-      <c r="B395" s="5"/>
+      <c r="A395" s="18"/>
+      <c r="B395" s="25"/>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="20"/>
-      <c r="B396" s="5"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="20"/>
-      <c r="B397" s="3"/>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="21"/>
-      <c r="B398" s="3"/>
+      <c r="A396" s="18"/>
+      <c r="B396" s="25"/>
+    </row>
+    <row r="397" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A397" s="18"/>
+      <c r="B397" s="22"/>
+    </row>
+    <row r="398" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A398" s="19"/>
+      <c r="B398" s="13" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="20"/>
-      <c r="B399" s="3"/>
+      <c r="A399" s="18"/>
+      <c r="B399" s="22"/>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="20"/>
-      <c r="B400" s="8"/>
+      <c r="A400" s="18"/>
+      <c r="B400" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="20"/>
-      <c r="B401" s="5"/>
+      <c r="A401" s="18"/>
+      <c r="B401" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="20"/>
-      <c r="B402" s="11"/>
+      <c r="A402" s="18"/>
+      <c r="B402" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="20"/>
-      <c r="B403" s="3"/>
+      <c r="A403" s="18"/>
+      <c r="B403" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="21"/>
-      <c r="B404" s="3"/>
+      <c r="A404" s="18"/>
+      <c r="B404" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="20"/>
-      <c r="B405" s="3"/>
+      <c r="A405" s="18"/>
+      <c r="B405" s="3" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="20"/>
-      <c r="B406" s="3"/>
+      <c r="A406" s="18"/>
+      <c r="B406" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="20"/>
-      <c r="B407" s="3"/>
+      <c r="A407" s="18"/>
+      <c r="B407" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="20"/>
-      <c r="B408" s="5"/>
+      <c r="A408" s="18"/>
+      <c r="B408" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="20"/>
-      <c r="B409" s="5"/>
+      <c r="A409" s="18"/>
+      <c r="B409" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="20"/>
-      <c r="B410" s="3"/>
+      <c r="A410" s="18"/>
+      <c r="B410" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="21"/>
-      <c r="B411" s="3"/>
+      <c r="A411" s="18"/>
+      <c r="B411" s="3" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="20"/>
-      <c r="B412" s="3"/>
+      <c r="A412" s="18"/>
+      <c r="B412" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="20"/>
-      <c r="B413" s="3"/>
+      <c r="A413" s="18"/>
+      <c r="B413" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="20"/>
-      <c r="B414" s="3"/>
+      <c r="A414" s="18"/>
+      <c r="B414" s="3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="20"/>
-      <c r="B415" s="3"/>
+      <c r="A415" s="18"/>
+      <c r="B415" s="3" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="20"/>
-      <c r="B416" s="3"/>
-    </row>
-    <row r="417" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A417" s="22"/>
-      <c r="B417" s="9"/>
+      <c r="A416" s="18"/>
+      <c r="B416" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="18"/>
+      <c r="B417" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="18"/>
+      <c r="B418" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="18"/>
+      <c r="B419" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" s="18"/>
+      <c r="B420" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" s="18"/>
+      <c r="B421" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" s="18"/>
+      <c r="B422" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" s="18"/>
+      <c r="B423" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" s="18"/>
+      <c r="B424" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" s="18"/>
+      <c r="B425" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" s="18"/>
+      <c r="B426" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" s="18"/>
+      <c r="B427" s="22"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" s="18"/>
+      <c r="B428" s="22"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" s="18"/>
+      <c r="B429" s="22"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" s="18"/>
+      <c r="B430" s="25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" s="18"/>
+      <c r="B431" s="25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="18"/>
+      <c r="B432" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="18"/>
+      <c r="B433" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="18"/>
+      <c r="B434" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="18"/>
+      <c r="B435" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="18"/>
+      <c r="B436" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="18"/>
+      <c r="B437" s="22"/>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="18"/>
+      <c r="B438" s="22"/>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="18"/>
+      <c r="B439" s="22"/>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="18"/>
+      <c r="B440" s="22"/>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="18"/>
+      <c r="B441" s="22"/>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="18"/>
+      <c r="B442" s="22"/>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="18"/>
+      <c r="B443" s="22"/>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="18"/>
+      <c r="B444" s="22"/>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="18"/>
+      <c r="B445" s="22"/>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="18"/>
+      <c r="B446" s="22"/>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="18"/>
+      <c r="B447" s="25"/>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="18"/>
+      <c r="B448" s="25"/>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" s="18"/>
+      <c r="B449" s="22"/>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" s="18"/>
+      <c r="B450" s="22"/>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" s="18"/>
+      <c r="B451" s="22"/>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" s="18"/>
+      <c r="B452" s="22"/>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" s="18"/>
+      <c r="B453" s="22"/>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" s="18"/>
+      <c r="B454" s="22"/>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" s="18"/>
+      <c r="B455" s="22"/>
+    </row>
+    <row r="456" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A456" s="20"/>
+      <c r="B456" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
-    <mergeCell ref="A316:A417"/>
+    <mergeCell ref="A316:A456"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o nome para form004.html e atualizada a planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDED46D-EF1E-49F6-B149-59A2CA02786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855CFE47-F888-4C35-9B9E-31F6C0005915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="272">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -13883,6 +13883,1385 @@
   </si>
   <si>
     <t>É muito importante fazer testes de funcionamento em vários navegadores diferentes!</t>
+  </si>
+  <si>
+    <t>7 – Formulários com telefone e email</t>
+  </si>
+  <si>
+    <t>Estudar expressões regulares ou RegEx</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Exemplo de formulário&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fieldset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>legend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Dados Pessoais&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>legend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Nome&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"nome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inome"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>minlength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>maxlength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"30"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iemail"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;E-mail&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iemail"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"itel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Telefone&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"itel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"^\(\d{2}\)\d{4,5}-\d{4}$"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>placeholder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"(xx)xxxx-xxxx"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"10"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fieldset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"reset"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Limpar"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O input tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para receber dados de email, o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete e-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para dar um alerta de erro caso o usuário não tenha colocado o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O input tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>tel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é um dos inputs para receber dados de telefone, o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para configurar o formato dos números, aí está como requerido e tem um </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>placeholder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> para destacar o formado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Os três tipos de dados estão envelopados dentro de um </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fieldset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, que serve para agrupar áreas de formulários e o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">legend </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>é a legenda do fieldset</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -14209,7 +15588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -14281,6 +15660,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -14293,9 +15675,11 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14659,10 +16043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:B451"/>
+  <dimension ref="A2:C499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B455" sqref="B455"/>
+    <sheetView tabSelected="1" topLeftCell="A466" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C489" sqref="C489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14682,7 +16066,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -14690,550 +16074,550 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
+      <c r="A54" s="31"/>
       <c r="B54" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="31"/>
       <c r="B55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="31"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="7"/>
     </row>
     <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
+      <c r="A75" s="31"/>
       <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="31"/>
       <c r="B78" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
+      <c r="A79" s="31"/>
       <c r="B79" s="7"/>
     </row>
     <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
+      <c r="A81" s="31"/>
       <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="31"/>
       <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
+      <c r="A83" s="31"/>
       <c r="B83" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="31"/>
       <c r="B84" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="30"/>
+      <c r="A85" s="31"/>
       <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="31"/>
+      <c r="A86" s="32"/>
       <c r="B86" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="31"/>
       <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="31"/>
       <c r="B88" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="30"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="31"/>
+      <c r="A92" s="32"/>
       <c r="B92" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
+      <c r="A96" s="31"/>
       <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="30"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="31"/>
+      <c r="A99" s="32"/>
       <c r="B99" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="30"/>
+      <c r="A104" s="31"/>
       <c r="B104" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="32"/>
+      <c r="A105" s="33"/>
       <c r="B105" s="9"/>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="29" t="s">
+      <c r="A109" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B109" s="13" t="s">
@@ -15241,1168 +16625,1168 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="30"/>
+      <c r="A110" s="31"/>
       <c r="B110" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
+      <c r="A111" s="31"/>
       <c r="B111" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="31"/>
       <c r="B112" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="31"/>
       <c r="B113" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="31"/>
       <c r="B114" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="31"/>
       <c r="B115" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="30"/>
+      <c r="A116" s="31"/>
       <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="31"/>
       <c r="B117" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="30"/>
+      <c r="A118" s="31"/>
       <c r="B118" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="31"/>
       <c r="B119" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="A120" s="31"/>
       <c r="B120" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="30"/>
+      <c r="A121" s="31"/>
       <c r="B121" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="31"/>
       <c r="B122" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="31"/>
       <c r="B123" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="31"/>
       <c r="B124" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="30"/>
+      <c r="A125" s="31"/>
       <c r="B125" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="31"/>
       <c r="B126" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="31"/>
       <c r="B127" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="30"/>
+      <c r="A128" s="31"/>
       <c r="B128" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="31"/>
       <c r="B129" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="31"/>
       <c r="B130" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="31"/>
       <c r="B131" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="30"/>
+      <c r="A132" s="31"/>
       <c r="B132" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="31"/>
       <c r="B133" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="30"/>
+      <c r="A134" s="31"/>
       <c r="B134" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="30"/>
+      <c r="A135" s="31"/>
       <c r="B135" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="30"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="30"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="30"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="3"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
+      <c r="A139" s="31"/>
       <c r="B139" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="30"/>
+      <c r="A140" s="31"/>
       <c r="B140" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="30"/>
+      <c r="A141" s="31"/>
       <c r="B141" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="30"/>
+      <c r="A142" s="31"/>
       <c r="B142" s="12" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="30"/>
+      <c r="A143" s="31"/>
       <c r="B143" s="12" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="30"/>
+      <c r="A144" s="31"/>
       <c r="B144" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="30"/>
+      <c r="A145" s="31"/>
       <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="30"/>
+      <c r="A146" s="31"/>
       <c r="B146" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="30"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
+      <c r="A148" s="31"/>
       <c r="B148" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
+      <c r="A149" s="31"/>
       <c r="B149" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="30"/>
+      <c r="A150" s="31"/>
       <c r="B150" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
+      <c r="A151" s="31"/>
       <c r="B151" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="30"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="30"/>
+      <c r="A153" s="31"/>
       <c r="B153" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="30"/>
+      <c r="A154" s="31"/>
       <c r="B154" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="30"/>
+      <c r="A155" s="31"/>
       <c r="B155" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="30"/>
+      <c r="A156" s="31"/>
       <c r="B156" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="30"/>
+      <c r="A157" s="31"/>
       <c r="B157" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="30"/>
+      <c r="A158" s="31"/>
       <c r="B158" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="30"/>
+      <c r="A159" s="31"/>
       <c r="B159" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="30"/>
+      <c r="A160" s="31"/>
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="30"/>
+      <c r="A161" s="31"/>
       <c r="B161" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="30"/>
+      <c r="A162" s="31"/>
       <c r="B162" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="30"/>
+      <c r="A163" s="31"/>
       <c r="B163" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="30"/>
+      <c r="A164" s="31"/>
       <c r="B164" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="30"/>
+      <c r="A165" s="31"/>
       <c r="B165" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="30"/>
+      <c r="A166" s="31"/>
       <c r="B166" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="30"/>
+      <c r="A167" s="31"/>
       <c r="B167" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="30"/>
+      <c r="A168" s="31"/>
       <c r="B168" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="30"/>
+      <c r="A169" s="31"/>
       <c r="B169" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="30"/>
+      <c r="A170" s="31"/>
       <c r="B170" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="30"/>
+      <c r="A171" s="31"/>
       <c r="B171" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="30"/>
+      <c r="A172" s="31"/>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="30"/>
+      <c r="A173" s="31"/>
       <c r="B173" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="30"/>
+      <c r="A174" s="31"/>
       <c r="B174" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="30"/>
+      <c r="A175" s="31"/>
       <c r="B175" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="30"/>
+      <c r="A176" s="31"/>
       <c r="B176" s="5"/>
     </row>
     <row r="177" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="30"/>
+      <c r="A177" s="31"/>
       <c r="B177" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="30"/>
+      <c r="A178" s="31"/>
       <c r="B178" s="5"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="30"/>
+      <c r="A179" s="31"/>
       <c r="B179" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="30"/>
+      <c r="A180" s="31"/>
       <c r="B180" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="30"/>
+      <c r="A181" s="31"/>
       <c r="B181" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="30"/>
+      <c r="A182" s="31"/>
       <c r="B182" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="30"/>
+      <c r="A183" s="31"/>
       <c r="B183" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="30"/>
+      <c r="A184" s="31"/>
       <c r="B184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="30"/>
+      <c r="A185" s="31"/>
       <c r="B185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="30"/>
+      <c r="A186" s="31"/>
       <c r="B186" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="30"/>
+      <c r="A187" s="31"/>
       <c r="B187" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="30"/>
+      <c r="A188" s="31"/>
       <c r="B188" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="30"/>
+      <c r="A189" s="31"/>
       <c r="B189" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="30"/>
+      <c r="A190" s="31"/>
       <c r="B190" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="30"/>
+      <c r="A191" s="31"/>
       <c r="B191" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="30"/>
+      <c r="A192" s="31"/>
       <c r="B192" s="5"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="30"/>
+      <c r="A193" s="31"/>
       <c r="B193" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="30"/>
+      <c r="A194" s="31"/>
       <c r="B194" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="30"/>
+      <c r="A195" s="31"/>
       <c r="B195" s="5"/>
     </row>
     <row r="196" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="30"/>
+      <c r="A196" s="31"/>
       <c r="B196" s="11" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="30"/>
+      <c r="A197" s="31"/>
       <c r="B197" s="15"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="30"/>
+      <c r="A198" s="31"/>
       <c r="B198" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="30"/>
+      <c r="A199" s="31"/>
       <c r="B199" s="7"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="30"/>
+      <c r="A200" s="31"/>
       <c r="B200" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="30"/>
+      <c r="A201" s="31"/>
       <c r="B201" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="30"/>
+      <c r="A202" s="31"/>
       <c r="B202" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="30"/>
+      <c r="A203" s="31"/>
       <c r="B203" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="30"/>
+      <c r="A204" s="31"/>
       <c r="B204" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="30"/>
+      <c r="A205" s="31"/>
       <c r="B205" s="16" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="30"/>
+      <c r="A206" s="31"/>
       <c r="B206" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="30"/>
+      <c r="A207" s="31"/>
       <c r="B207" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="30"/>
+      <c r="A208" s="31"/>
       <c r="B208" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="30"/>
+      <c r="A209" s="31"/>
       <c r="B209" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="30"/>
+      <c r="A210" s="31"/>
       <c r="B210" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="30"/>
+      <c r="A211" s="31"/>
       <c r="B211" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="30"/>
+      <c r="A212" s="31"/>
       <c r="B212" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="30"/>
+      <c r="A213" s="31"/>
       <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="30"/>
+      <c r="A214" s="31"/>
       <c r="B214" s="14" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="30"/>
+      <c r="A215" s="31"/>
       <c r="B215" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="30"/>
+      <c r="A216" s="31"/>
       <c r="B216" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="30"/>
+      <c r="A217" s="31"/>
       <c r="B217" s="3" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="30"/>
+      <c r="A218" s="31"/>
       <c r="B218" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="30"/>
+      <c r="A219" s="31"/>
       <c r="B219" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="30"/>
+      <c r="A220" s="31"/>
       <c r="B220" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="30"/>
+      <c r="A221" s="31"/>
       <c r="B221" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="30"/>
+      <c r="A222" s="31"/>
       <c r="B222" s="7"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="30"/>
+      <c r="A223" s="31"/>
       <c r="B223" s="14" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="30"/>
+      <c r="A224" s="31"/>
       <c r="B224" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="30"/>
+      <c r="A225" s="31"/>
       <c r="B225" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="30"/>
+      <c r="A226" s="31"/>
       <c r="B226" s="5"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="30"/>
+      <c r="A227" s="31"/>
       <c r="B227" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="30"/>
+      <c r="A228" s="31"/>
       <c r="B228" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="30"/>
+      <c r="A229" s="31"/>
       <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="30"/>
+      <c r="A230" s="31"/>
       <c r="B230" s="11" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="30"/>
+      <c r="A231" s="31"/>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="30"/>
+      <c r="A232" s="31"/>
       <c r="B232" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="30"/>
+      <c r="A233" s="31"/>
       <c r="B233" s="7"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="30"/>
+      <c r="A234" s="31"/>
       <c r="B234" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="30"/>
+      <c r="A235" s="31"/>
       <c r="B235" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="30"/>
+      <c r="A236" s="31"/>
       <c r="B236" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="30"/>
+      <c r="A237" s="31"/>
       <c r="B237" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="30"/>
+      <c r="A238" s="31"/>
       <c r="B238" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="30"/>
+      <c r="A239" s="31"/>
       <c r="B239" s="7"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="30"/>
+      <c r="A240" s="31"/>
       <c r="B240" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="30"/>
+      <c r="A241" s="31"/>
       <c r="B241" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="30"/>
+      <c r="A242" s="31"/>
       <c r="B242" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="30"/>
+      <c r="A243" s="31"/>
       <c r="B243" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="30"/>
+      <c r="A244" s="31"/>
       <c r="B244" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="30"/>
+      <c r="A245" s="31"/>
       <c r="B245" s="7"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="30"/>
+      <c r="A246" s="31"/>
       <c r="B246" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="30"/>
+      <c r="A247" s="31"/>
       <c r="B247" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="30"/>
+      <c r="A248" s="31"/>
       <c r="B248" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="30"/>
+      <c r="A249" s="31"/>
       <c r="B249" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="30"/>
+      <c r="A250" s="31"/>
       <c r="B250" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="30"/>
+      <c r="A251" s="31"/>
       <c r="B251" s="7"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="30"/>
+      <c r="A252" s="31"/>
       <c r="B252" s="14" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="30"/>
+      <c r="A253" s="31"/>
       <c r="B253" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="30"/>
+      <c r="A254" s="31"/>
       <c r="B254" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="30"/>
+      <c r="A255" s="31"/>
       <c r="B255" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="30"/>
+      <c r="A256" s="31"/>
       <c r="B256" s="7"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="30"/>
+      <c r="A257" s="31"/>
       <c r="B257" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="30"/>
+      <c r="A258" s="31"/>
       <c r="B258" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="30"/>
+      <c r="A259" s="31"/>
       <c r="B259" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="30"/>
+      <c r="A260" s="31"/>
       <c r="B260" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="30"/>
+      <c r="A261" s="31"/>
       <c r="B261" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="30"/>
+      <c r="A262" s="31"/>
       <c r="B262" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="30"/>
+      <c r="A263" s="31"/>
       <c r="B263" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="30"/>
+      <c r="A264" s="31"/>
       <c r="B264" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="30"/>
+      <c r="A265" s="31"/>
       <c r="B265" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="30"/>
+      <c r="A266" s="31"/>
       <c r="B266" s="7"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="30"/>
+      <c r="A267" s="31"/>
       <c r="B267" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="30"/>
+      <c r="A268" s="31"/>
       <c r="B268" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="30"/>
+      <c r="A269" s="31"/>
       <c r="B269" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="30"/>
+      <c r="A270" s="31"/>
       <c r="B270" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="30"/>
+      <c r="A271" s="31"/>
       <c r="B271" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="30"/>
+      <c r="A272" s="31"/>
       <c r="B272" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="30"/>
+      <c r="A273" s="31"/>
       <c r="B273" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="30"/>
+      <c r="A274" s="31"/>
       <c r="B274" s="7"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="30"/>
+      <c r="A275" s="31"/>
       <c r="B275" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="30"/>
+      <c r="A276" s="31"/>
       <c r="B276" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="30"/>
+      <c r="A277" s="31"/>
       <c r="B277" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="30"/>
+      <c r="A278" s="31"/>
       <c r="B278" s="7"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="30"/>
+      <c r="A279" s="31"/>
       <c r="B279" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="30"/>
+      <c r="A280" s="31"/>
       <c r="B280" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="30"/>
+      <c r="A281" s="31"/>
       <c r="B281" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="30"/>
+      <c r="A282" s="31"/>
       <c r="B282" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="30"/>
+      <c r="A283" s="31"/>
       <c r="B283" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="30"/>
+      <c r="A284" s="31"/>
       <c r="B284" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="30"/>
+      <c r="A285" s="31"/>
       <c r="B285" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="30"/>
+      <c r="A286" s="31"/>
       <c r="B286" s="7"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="30"/>
+      <c r="A287" s="31"/>
       <c r="B287" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="30"/>
+      <c r="A288" s="31"/>
       <c r="B288" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="30"/>
+      <c r="A289" s="31"/>
       <c r="B289" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="30"/>
+      <c r="A290" s="31"/>
       <c r="B290" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="30"/>
+      <c r="A291" s="31"/>
       <c r="B291" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="30"/>
+      <c r="A292" s="31"/>
       <c r="B292" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="30"/>
+      <c r="A293" s="31"/>
       <c r="B293" s="5"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="30"/>
+      <c r="A294" s="31"/>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="30"/>
+      <c r="A295" s="31"/>
       <c r="B295" s="5"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="30"/>
+      <c r="A296" s="31"/>
       <c r="B296" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="30"/>
+      <c r="A297" s="31"/>
       <c r="B297" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="30"/>
+      <c r="A298" s="31"/>
       <c r="B298" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="30"/>
+      <c r="A299" s="31"/>
       <c r="B299" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="30"/>
+      <c r="A300" s="31"/>
       <c r="B300" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="30"/>
+      <c r="A301" s="31"/>
       <c r="B301" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="30"/>
+      <c r="A302" s="31"/>
       <c r="B302" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="30"/>
+      <c r="A303" s="31"/>
       <c r="B303" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="30"/>
+      <c r="A304" s="31"/>
       <c r="B304" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="30"/>
+      <c r="A305" s="31"/>
       <c r="B305" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="30"/>
+      <c r="A306" s="31"/>
       <c r="B306" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="30"/>
+      <c r="A307" s="31"/>
       <c r="B307" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="30"/>
+      <c r="A308" s="31"/>
       <c r="B308" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="30"/>
+      <c r="A309" s="31"/>
       <c r="B309" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="30"/>
+      <c r="A310" s="31"/>
       <c r="B310" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="30"/>
+      <c r="A311" s="31"/>
       <c r="B311" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="32"/>
+      <c r="A312" s="33"/>
       <c r="B312" s="9"/>
     </row>
     <row r="315" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="316" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A316" s="29" t="s">
+      <c r="A316" s="30" t="s">
         <v>199</v>
       </c>
       <c r="B316" s="13" t="s">
@@ -16410,726 +17794,995 @@
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="30"/>
+      <c r="A317" s="31"/>
       <c r="B317" s="17"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="30"/>
+      <c r="A318" s="31"/>
       <c r="B318" s="18"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="30"/>
+      <c r="A319" s="31"/>
       <c r="B319" s="19"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="30"/>
+      <c r="A320" s="31"/>
       <c r="B320" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="30"/>
+      <c r="A321" s="31"/>
       <c r="B321" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="30"/>
+      <c r="A322" s="31"/>
       <c r="B322" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="30"/>
+      <c r="A323" s="31"/>
       <c r="B323" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="30"/>
+      <c r="A324" s="31"/>
       <c r="B324" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="30"/>
+      <c r="A325" s="31"/>
       <c r="B325" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="30"/>
+      <c r="A326" s="31"/>
       <c r="B326" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="30"/>
+      <c r="A327" s="31"/>
       <c r="B327" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="30"/>
+      <c r="A328" s="31"/>
       <c r="B328" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="30"/>
+      <c r="A329" s="31"/>
       <c r="B329" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="30"/>
+      <c r="A330" s="31"/>
       <c r="B330" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="30"/>
+      <c r="A331" s="31"/>
       <c r="B331" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="30"/>
+      <c r="A332" s="31"/>
       <c r="B332" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="30"/>
+      <c r="A333" s="31"/>
       <c r="B333" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="30"/>
+      <c r="A334" s="31"/>
       <c r="B334" s="3" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="30"/>
+      <c r="A335" s="31"/>
       <c r="B335" s="3" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="30"/>
+      <c r="A336" s="31"/>
       <c r="B336" s="3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="30"/>
+      <c r="A337" s="31"/>
       <c r="B337" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="30"/>
+      <c r="A338" s="31"/>
       <c r="B338" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="30"/>
+      <c r="A339" s="31"/>
       <c r="B339" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="30"/>
+      <c r="A340" s="31"/>
       <c r="B340" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="30"/>
+      <c r="A341" s="31"/>
       <c r="B341" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="30"/>
+      <c r="A342" s="31"/>
       <c r="B342" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="30"/>
+      <c r="A343" s="31"/>
       <c r="B343" s="3"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="30"/>
+      <c r="A344" s="31"/>
       <c r="B344" s="20"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="30"/>
+      <c r="A345" s="31"/>
       <c r="B345" s="18"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="30"/>
+      <c r="A346" s="31"/>
       <c r="B346" s="18"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="30"/>
+      <c r="A347" s="31"/>
       <c r="B347" s="21" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" s="30"/>
+      <c r="A348" s="31"/>
       <c r="B348" s="21" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="30"/>
+      <c r="A349" s="31"/>
       <c r="B349" s="22" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" s="30"/>
+      <c r="A350" s="31"/>
       <c r="B350" s="21" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" s="30"/>
+      <c r="A351" s="31"/>
       <c r="B351" s="23" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" s="30"/>
+      <c r="A352" s="31"/>
       <c r="B352" s="23" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A353" s="30"/>
+      <c r="A353" s="31"/>
       <c r="B353" s="21"/>
     </row>
     <row r="354" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A354" s="31"/>
+      <c r="A354" s="32"/>
       <c r="B354" s="13" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="30"/>
+      <c r="A355" s="31"/>
       <c r="B355" s="21"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" s="30"/>
+      <c r="A356" s="31"/>
       <c r="B356" s="21" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" s="30"/>
+      <c r="A357" s="31"/>
       <c r="B357" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="30"/>
+      <c r="A358" s="31"/>
       <c r="B358" s="24" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="30"/>
+      <c r="A359" s="31"/>
       <c r="B359" s="25" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="30"/>
+      <c r="A360" s="31"/>
       <c r="B360" s="18" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="30"/>
+      <c r="A361" s="31"/>
       <c r="B361" s="25" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="30"/>
+      <c r="A362" s="31"/>
       <c r="B362" s="26" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="30"/>
+      <c r="A363" s="31"/>
       <c r="B363" s="18"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="30"/>
+      <c r="A364" s="31"/>
       <c r="B364" s="21"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="30"/>
+      <c r="A365" s="31"/>
       <c r="B365" s="21"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="30"/>
+      <c r="A366" s="31"/>
       <c r="B366" s="28"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="30"/>
+      <c r="A367" s="31"/>
       <c r="B367" s="28"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="30"/>
+      <c r="A368" s="31"/>
       <c r="B368" s="5"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="30"/>
+      <c r="A369" s="31"/>
       <c r="B369" s="18"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="30"/>
+      <c r="A370" s="31"/>
       <c r="B370" s="21"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="30"/>
+      <c r="A371" s="31"/>
       <c r="B371" s="18"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="30"/>
+      <c r="A372" s="31"/>
       <c r="B372" s="24"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="30"/>
+      <c r="A373" s="31"/>
       <c r="B373" s="20"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="30"/>
+      <c r="A374" s="31"/>
       <c r="B374" s="18"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="30"/>
+      <c r="A375" s="31"/>
       <c r="B375" s="18"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="30"/>
+      <c r="A376" s="31"/>
       <c r="B376" s="18"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="30"/>
+      <c r="A377" s="31"/>
       <c r="B377" s="18"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="30"/>
+      <c r="A378" s="31"/>
       <c r="B378" s="18"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="30"/>
+      <c r="A379" s="31"/>
       <c r="B379" s="18"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="30"/>
+      <c r="A380" s="31"/>
       <c r="B380" s="18"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="30"/>
+      <c r="A381" s="31"/>
       <c r="B381" s="18"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="30"/>
+      <c r="A382" s="31"/>
       <c r="B382" s="18"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="30"/>
+      <c r="A383" s="31"/>
       <c r="B383" s="18"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="30"/>
+      <c r="A384" s="31"/>
       <c r="B384" s="18"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="30"/>
+      <c r="A385" s="31"/>
       <c r="B385" s="20"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="30"/>
+      <c r="A386" s="31"/>
       <c r="B386" s="24"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="30"/>
+      <c r="A387" s="31"/>
       <c r="B387" s="20"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="30"/>
+      <c r="A388" s="31"/>
       <c r="B388" s="18"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="30"/>
+      <c r="A389" s="31"/>
       <c r="B389" s="18"/>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="30"/>
+      <c r="A390" s="31"/>
       <c r="B390" s="18"/>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="30"/>
+      <c r="A391" s="31"/>
       <c r="B391" s="20"/>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="30"/>
+      <c r="A392" s="31"/>
       <c r="B392" s="24"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="30"/>
+      <c r="A393" s="31"/>
       <c r="B393" s="18"/>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="30"/>
+      <c r="A394" s="31"/>
       <c r="B394" s="21"/>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="30"/>
+      <c r="A395" s="31"/>
       <c r="B395" s="21"/>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="30"/>
+      <c r="A396" s="31"/>
       <c r="B396" s="21"/>
     </row>
     <row r="397" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="30"/>
+      <c r="A397" s="31"/>
       <c r="B397" s="18"/>
     </row>
     <row r="398" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A398" s="31"/>
+      <c r="A398" s="32"/>
       <c r="B398" s="13" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="30"/>
+      <c r="A399" s="31"/>
       <c r="B399" s="18"/>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="30"/>
+      <c r="A400" s="31"/>
       <c r="B400" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="30"/>
+      <c r="A401" s="31"/>
       <c r="B401" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="30"/>
+      <c r="A402" s="31"/>
       <c r="B402" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="30"/>
+      <c r="A403" s="31"/>
       <c r="B403" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="30"/>
+      <c r="A404" s="31"/>
       <c r="B404" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="30"/>
+      <c r="A405" s="31"/>
       <c r="B405" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="30"/>
+      <c r="A406" s="31"/>
       <c r="B406" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="30"/>
+      <c r="A407" s="31"/>
       <c r="B407" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="30"/>
+      <c r="A408" s="31"/>
       <c r="B408" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="30"/>
+      <c r="A409" s="31"/>
       <c r="B409" s="3" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="30"/>
+      <c r="A410" s="31"/>
       <c r="B410" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="30"/>
+      <c r="A411" s="31"/>
       <c r="B411" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="30"/>
+      <c r="A412" s="31"/>
       <c r="B412" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="30"/>
+      <c r="A413" s="31"/>
       <c r="B413" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="30"/>
+      <c r="A414" s="31"/>
       <c r="B414" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="30"/>
+      <c r="A415" s="31"/>
       <c r="B415" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="30"/>
+      <c r="A416" s="31"/>
       <c r="B416" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="30"/>
+      <c r="A417" s="31"/>
       <c r="B417" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="30"/>
+      <c r="A418" s="31"/>
       <c r="B418" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="30"/>
+      <c r="A419" s="31"/>
       <c r="B419" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="30"/>
+      <c r="A420" s="31"/>
       <c r="B420" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="30"/>
+      <c r="A421" s="31"/>
       <c r="B421" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="30"/>
+      <c r="A422" s="31"/>
       <c r="B422" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="30"/>
+      <c r="A423" s="31"/>
       <c r="B423" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="30"/>
+      <c r="A424" s="31"/>
       <c r="B424" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="30"/>
+      <c r="A425" s="31"/>
       <c r="B425" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A426" s="30"/>
+      <c r="A426" s="31"/>
       <c r="B426" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="30"/>
+      <c r="A427" s="31"/>
       <c r="B427" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A428" s="30"/>
+      <c r="A428" s="31"/>
       <c r="B428" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A429" s="30"/>
+      <c r="A429" s="31"/>
       <c r="B429" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A430" s="30"/>
+      <c r="A430" s="31"/>
       <c r="B430" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A431" s="30"/>
+      <c r="A431" s="31"/>
       <c r="B431" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A432" s="30"/>
+      <c r="A432" s="31"/>
       <c r="B432" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="30"/>
+      <c r="A433" s="31"/>
       <c r="B433" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="30"/>
+      <c r="A434" s="31"/>
       <c r="B434" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="30"/>
+      <c r="A435" s="31"/>
       <c r="B435" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="30"/>
+      <c r="A436" s="31"/>
       <c r="B436" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="30"/>
+      <c r="A437" s="31"/>
       <c r="B437" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="30"/>
+      <c r="A438" s="31"/>
       <c r="B438" s="18"/>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="30"/>
+      <c r="A439" s="31"/>
       <c r="B439" s="21" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A440" s="30"/>
+      <c r="A440" s="31"/>
       <c r="B440" s="21" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A441" s="30"/>
+      <c r="A441" s="31"/>
       <c r="B441" s="18" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A442" s="30"/>
+      <c r="A442" s="31"/>
       <c r="B442" s="18" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A443" s="30"/>
+      <c r="A443" s="31"/>
       <c r="B443" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A444" s="30"/>
+      <c r="A444" s="31"/>
       <c r="B444" s="18" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A445" s="30"/>
+      <c r="A445" s="31"/>
       <c r="B445" s="18" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="30"/>
+      <c r="A446" s="31"/>
       <c r="B446" s="18" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="30"/>
+      <c r="A447" s="31"/>
       <c r="B447" s="18" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="30"/>
+      <c r="A448" s="31"/>
       <c r="B448" s="18" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="30"/>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" s="31"/>
       <c r="B449" s="18" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="450" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A450" s="30"/>
-      <c r="B450" s="33" t="s">
+    <row r="450" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A450" s="31"/>
+      <c r="B450" s="29" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="451" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A451" s="32"/>
-      <c r="B451" s="27"/>
+    <row r="451" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A451" s="31"/>
+      <c r="B451" s="9"/>
+    </row>
+    <row r="452" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A452" s="32"/>
+      <c r="B452" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A453" s="31"/>
+      <c r="C453" s="36"/>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A454" s="31"/>
+      <c r="B454" s="35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" s="31"/>
+      <c r="B455" s="28"/>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" s="31"/>
+      <c r="B456" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A457" s="31"/>
+      <c r="B457" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A458" s="31"/>
+      <c r="B458" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A459" s="31"/>
+      <c r="B459" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A460" s="31"/>
+      <c r="B460" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A461" s="31"/>
+      <c r="B461" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A462" s="31"/>
+      <c r="B462" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A463" s="31"/>
+      <c r="B463" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A464" s="31"/>
+      <c r="B464" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="C464" s="36"/>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" s="31"/>
+      <c r="B465" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" s="31"/>
+      <c r="B466" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" s="31"/>
+      <c r="B467" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A468" s="31"/>
+      <c r="B468" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A469" s="31"/>
+      <c r="B469" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" s="31"/>
+      <c r="B470" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C470" s="36"/>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A471" s="31"/>
+      <c r="B471" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A472" s="31"/>
+      <c r="B472" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" s="31"/>
+      <c r="B473" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="C473" s="36"/>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A474" s="31"/>
+      <c r="B474" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A475" s="31"/>
+      <c r="B475" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" s="31"/>
+      <c r="B476" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A477" s="31"/>
+      <c r="B477" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A478" s="31"/>
+      <c r="B478" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" s="31"/>
+      <c r="B479" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" s="31"/>
+      <c r="B480" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A481" s="31"/>
+      <c r="B481" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" s="31"/>
+      <c r="B482" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A483" s="31"/>
+      <c r="B483" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A484" s="31"/>
+      <c r="B484" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" s="31"/>
+      <c r="B485" s="7"/>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A486" s="31"/>
+      <c r="B486" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A487" s="31"/>
+      <c r="B487" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" s="31"/>
+      <c r="B488" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A489" s="31"/>
+      <c r="C489" s="36"/>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A490" s="31"/>
+      <c r="B490" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" s="31"/>
+      <c r="B491" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A492" s="31"/>
+      <c r="B492" s="18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A493" s="31"/>
+      <c r="B493" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A494" s="31"/>
+      <c r="B494" s="18"/>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A495" s="31"/>
+      <c r="B495" s="18"/>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496" s="31"/>
+      <c r="C496" s="36"/>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" s="31"/>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" s="31"/>
+    </row>
+    <row r="499" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A499" s="33"/>
+      <c r="B499" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
-    <mergeCell ref="A316:A451"/>
+    <mergeCell ref="A316:A499"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o form006 e atualizei a planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B36A5-559F-4680-82B6-EB496AC6592F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7CAAF3-3632-4BEE-B6F7-7294BD8C9E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="295">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -16831,6 +16831,1068 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> serve para marcar várias opções diferentes</t>
+    </r>
+  </si>
+  <si>
+    <t>Aula 9 – Color, range e file</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"cadastro.php"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"post"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"on"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"icor"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Cor:&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"color"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"cor"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"icor"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"#00ff00"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inivel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Nível de Satisfação: &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"range"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"nivel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"inivel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"100"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ifoto"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Foto do Perfil:&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"file"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"foto"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ifoto"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O input tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para abrir uma caixa para seleção de cores e o value é para selecionar uma cor específica padrão que irá aparecer no site.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O input tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> serve para abrir uma caixa com seletor de nível que pode variar conforme o valor colocado no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, o valor é o padrão conforme acima</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O input tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é para abrir um botão para carregar uma foto do computador. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>****Lembrando que quando utilizar esse input, deve-se mudar para o</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> method post</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> devido ultrapassar os 3kb****</t>
     </r>
   </si>
 </sst>
@@ -16838,7 +17900,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16994,6 +18056,24 @@
       <b/>
       <i/>
       <sz val="12"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFE1E1E6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -17613,10 +18693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:C547"/>
+  <dimension ref="A2:C577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A493" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B528" sqref="B528"/>
+    <sheetView tabSelected="1" topLeftCell="A547" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20530,87 +21610,275 @@
         <v>282</v>
       </c>
     </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" s="34"/>
       <c r="B529" s="18" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A530" s="34"/>
       <c r="B530" s="18"/>
     </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A531" s="34"/>
-      <c r="B531" s="18"/>
-    </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B531" s="13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" s="34"/>
-      <c r="B532" s="18"/>
-    </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B532" s="1"/>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" s="34"/>
-      <c r="B533" s="18"/>
-    </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B533" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" s="34"/>
-      <c r="B534" s="18"/>
-    </row>
-    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B534" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" s="34"/>
-      <c r="B535" s="18"/>
-    </row>
-    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B535" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" s="34"/>
-      <c r="B536" s="18"/>
-    </row>
-    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B536" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" s="34"/>
-      <c r="B537" s="18"/>
-    </row>
-    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B537" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" s="34"/>
-      <c r="B538" s="18"/>
-    </row>
-    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B538" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" s="34"/>
-      <c r="B539" s="18"/>
-    </row>
-    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B539" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" s="34"/>
-      <c r="B540" s="18"/>
-    </row>
-    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B540" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" s="34"/>
-      <c r="B541" s="18"/>
-    </row>
-    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B541" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" s="34"/>
-      <c r="B542" s="18"/>
-    </row>
-    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B542" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" s="34"/>
-      <c r="B543" s="18"/>
-    </row>
-    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B543" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" s="34"/>
-      <c r="C544" s="32"/>
+      <c r="B544" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" s="34"/>
+      <c r="B545" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" s="34"/>
-    </row>
-    <row r="547" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="36"/>
-      <c r="B547" s="27"/>
+      <c r="B546" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A547" s="34"/>
+      <c r="B547" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" s="34"/>
+      <c r="B548" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" s="34"/>
+      <c r="B549" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A550" s="34"/>
+      <c r="B550" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A551" s="34"/>
+      <c r="B551" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" s="34"/>
+      <c r="B552" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" s="34"/>
+      <c r="B553" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" s="34"/>
+      <c r="B554" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A555" s="34"/>
+      <c r="B555" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" s="34"/>
+      <c r="B556" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" s="34"/>
+      <c r="B557" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A558" s="34"/>
+      <c r="B558" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A559" s="34"/>
+      <c r="B559" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" s="34"/>
+      <c r="B560" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A561" s="34"/>
+      <c r="B561" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A562" s="34"/>
+      <c r="B562" s="18"/>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" s="34"/>
+      <c r="B563" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" s="34"/>
+      <c r="B564" s="21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A565" s="34"/>
+      <c r="B565" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" s="34"/>
+      <c r="B566" s="18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A567" s="34"/>
+      <c r="B567" s="18"/>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A568" s="34"/>
+      <c r="B568" s="18"/>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" s="34"/>
+      <c r="B569" s="18"/>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A570" s="34"/>
+      <c r="B570" s="18"/>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A571" s="34"/>
+      <c r="B571" s="18"/>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572" s="34"/>
+      <c r="B572" s="18"/>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A573" s="34"/>
+      <c r="B573" s="18"/>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A574" s="34"/>
+      <c r="C574" s="32"/>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A575" s="34"/>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A576" s="34"/>
+    </row>
+    <row r="577" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A577" s="36"/>
+      <c r="B577" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
-    <mergeCell ref="A316:A547"/>
+    <mergeCell ref="A316:A577"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado form007 e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\html-e-css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7CAAF3-3632-4BEE-B6F7-7294BD8C9E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA2FC20-A429-45E1-A95D-C31101392FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="321">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -17893,6 +17893,1706 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> devido ultrapassar os 3kb****</t>
+    </r>
+  </si>
+  <si>
+    <t>10 – Select, datalist e textarea</t>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iest"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Estado&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estado"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iest"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>selected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;----- Escolha -----&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>optgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Região Sul"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"PR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Paraná&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"SC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Santa Catarina&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"RS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Rio Grande do Sul&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>optgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>optgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Região Sudeste"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"MG"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Minas Gerais&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"RJ"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Rio de Janeiro&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"SP"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;São Paulo&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iprof"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Profissão&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"prof"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"iprof"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"lstprof"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>datalist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"lstprof"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Administrador&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Contabilista&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Desenvolvedor&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Professor&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;!--&lt;option value="PROF"&gt;Professor&lt;/option&gt;--&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>datalist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;            </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"imsg"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Mensagem&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>textarea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"msg"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"imsg"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cols</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"30"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"10"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>textarea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;!--Textarea tem que usar o method post, por conta dos 3000 palavras..--&gt;</t>
     </r>
   </si>
 </sst>
@@ -17900,7 +19600,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18077,6 +19777,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5A4B81"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -18238,7 +19944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -18329,6 +20035,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18693,16 +20402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:C577"/>
+  <dimension ref="A2:C631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A547" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+    <sheetView tabSelected="1" topLeftCell="A573" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B626" sqref="B626"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="225" style="4" customWidth="1"/>
+    <col min="2" max="2" width="252.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -21798,87 +23507,405 @@
         <v>33</v>
       </c>
     </row>
-    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" s="34"/>
       <c r="B561" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" s="34"/>
       <c r="B562" s="18"/>
     </row>
-    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" s="34"/>
       <c r="B563" s="21" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" s="34"/>
       <c r="B564" s="21" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" s="34"/>
       <c r="B565" s="18" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" s="34"/>
       <c r="B566" s="18" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A567" s="34"/>
       <c r="B567" s="18"/>
     </row>
-    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A568" s="34"/>
-      <c r="B568" s="18"/>
-    </row>
-    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B568" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" s="34"/>
       <c r="B569" s="18"/>
     </row>
-    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" s="34"/>
-      <c r="B570" s="18"/>
-    </row>
-    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B570" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" s="34"/>
-      <c r="B571" s="18"/>
-    </row>
-    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B571" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" s="34"/>
-      <c r="B572" s="18"/>
-    </row>
-    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B572" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" s="34"/>
-      <c r="B573" s="18"/>
-    </row>
-    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B573" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" s="34"/>
-      <c r="C574" s="32"/>
-    </row>
-    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B574" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" s="34"/>
-    </row>
-    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B575" s="30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" s="34"/>
-    </row>
-    <row r="577" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A577" s="36"/>
-      <c r="B577" s="27"/>
+      <c r="B576" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" s="34"/>
+      <c r="B577" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" s="34"/>
+      <c r="B578" s="30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" s="34"/>
+      <c r="B579" s="30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" s="34"/>
+      <c r="B580" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A581" s="34"/>
+      <c r="B581" s="30" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A582" s="34"/>
+      <c r="B582" s="30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" s="34"/>
+      <c r="B583" s="30" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A584" s="34"/>
+      <c r="B584" s="30" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A585" s="34"/>
+      <c r="B585" s="30" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A586" s="34"/>
+      <c r="B586" s="30" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A587" s="34"/>
+      <c r="B587" s="30" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A588" s="34"/>
+      <c r="B588" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A589" s="34"/>
+      <c r="B589" s="37"/>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A590" s="34"/>
+      <c r="B590" s="30" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A591" s="34"/>
+      <c r="B591" s="30" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A592" s="34"/>
+      <c r="B592" s="30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A593" s="34"/>
+      <c r="B593" s="30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A594" s="34"/>
+      <c r="B594" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" s="34"/>
+      <c r="B595" s="30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" s="34"/>
+      <c r="B596" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" s="34"/>
+      <c r="B597" s="37"/>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" s="34"/>
+      <c r="B598" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" s="34"/>
+      <c r="B599" s="30" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" s="34"/>
+      <c r="B600" s="30" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" s="34"/>
+      <c r="B601" s="30" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" s="34"/>
+      <c r="B602" s="30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" s="34"/>
+      <c r="B603" s="30" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" s="34"/>
+      <c r="B604" s="30" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" s="34"/>
+      <c r="B605" s="30" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" s="34"/>
+      <c r="B606" s="30" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" s="34"/>
+      <c r="B607" s="30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" s="34"/>
+      <c r="B608" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" s="34"/>
+      <c r="B609" s="37"/>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" s="34"/>
+      <c r="B610" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" s="34"/>
+      <c r="B611" s="30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" s="34"/>
+      <c r="B612" s="30" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" s="34"/>
+      <c r="B613" s="30" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" s="34"/>
+      <c r="B614" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" s="34"/>
+      <c r="B615" s="37"/>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" s="34"/>
+      <c r="B616" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" s="34"/>
+      <c r="B617" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" s="34"/>
+      <c r="B618" s="30" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" s="34"/>
+      <c r="B619" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" s="34"/>
+      <c r="B620" s="30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" s="34"/>
+      <c r="B621" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" s="34"/>
+      <c r="B622" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" s="34"/>
+      <c r="B623" s="18"/>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" s="34"/>
+      <c r="B624" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" s="34"/>
+      <c r="B625" s="21"/>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" s="34"/>
+      <c r="B626" s="18"/>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" s="34"/>
+      <c r="B627" s="18"/>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A628" s="34"/>
+      <c r="C628" s="32"/>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" s="34"/>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630" s="34"/>
+    </row>
+    <row r="631" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A631" s="36"/>
+      <c r="B631" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
-    <mergeCell ref="A316:A577"/>
+    <mergeCell ref="A316:A631"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ex002 de Media Query
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D564DEAC-AC36-448F-80F3-BCC067864E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B660E-D204-4FF8-9FCF-DBE6AB1D13C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="411">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -24546,6 +24546,20 @@
     <t>E o tela.css que é o padrão de formatação para a tela, neste caso somente de dispositivo normal.. ****Exemplo de MEDIA TYPES****</t>
   </si>
   <si>
+    <t>Aula 03 – Múltiplas Media Features</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Media Query = Media Types + Media Features. </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -24555,7 +24569,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Media Query = Media Types + Media Features.  </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -24569,12 +24583,551 @@
       <t xml:space="preserve">              Aula 02 – Preparando um site para impressão</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Mude a orientação do seu dispositivo&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/paisagem.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"screen and (orientation: landscape)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt;   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">*** Configurações para todas as telas em modo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>paisagem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/retrato.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"screen and (orientation: portrait)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt;   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">*** Configurações para todas as telas em modo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>retrato</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ***</t>
+    </r>
+  </si>
+  <si>
+    <t>As Medias Types não tem parênteses</t>
+  </si>
+  <si>
+    <t>As Medias Features são informadas as características dentro de parênteses ISOLADAMENTE, Se tiver 3 Media Features, deverá informar cada característica em parênteses, no caso 3.</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/style.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"all"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt;   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">*** Configurações para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>todos os tipos de Medias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ***</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -24791,6 +25344,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -25483,10 +26053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:C878"/>
+  <dimension ref="A2:C955"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A769" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B776" sqref="B776"/>
+    <sheetView tabSelected="1" topLeftCell="A877" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B882" sqref="B882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29760,7 +30330,7 @@
         <v>346</v>
       </c>
       <c r="B778" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="779" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30316,20 +30886,362 @@
         <v>106</v>
       </c>
     </row>
-    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A877" s="43"/>
-      <c r="B877" s="24"/>
-    </row>
-    <row r="878" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A878" s="45"/>
-      <c r="B878" s="40"/>
+      <c r="B877" s="18"/>
+    </row>
+    <row r="878" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A878" s="44"/>
+      <c r="B878" s="13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A879" s="43"/>
+      <c r="B879" s="18"/>
+    </row>
+    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A880" s="43"/>
+      <c r="B880" s="18"/>
+    </row>
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A881" s="43"/>
+      <c r="B881" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A882" s="43"/>
+      <c r="B882" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A883" s="43"/>
+      <c r="B883" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" s="43"/>
+      <c r="B884" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" s="43"/>
+      <c r="B885" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" s="43"/>
+      <c r="B886" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A887" s="43"/>
+      <c r="B887" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A888" s="43"/>
+      <c r="B888" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A889" s="43"/>
+      <c r="B889" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A890" s="43"/>
+      <c r="B890" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A891" s="43"/>
+      <c r="B891" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A892" s="43"/>
+      <c r="B892" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A893" s="43"/>
+      <c r="B893" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A894" s="43"/>
+      <c r="B894" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A895" s="43"/>
+      <c r="B895" s="3"/>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A896" s="43"/>
+      <c r="B896" s="21" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A897" s="43"/>
+      <c r="B897" s="18" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A898" s="43"/>
+      <c r="B898" s="18"/>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A899" s="43"/>
+      <c r="B899" s="18"/>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A900" s="43"/>
+      <c r="B900" s="18"/>
+    </row>
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A901" s="43"/>
+      <c r="B901" s="18"/>
+    </row>
+    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A902" s="43"/>
+      <c r="B902" s="18"/>
+    </row>
+    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A903" s="43"/>
+      <c r="B903" s="18"/>
+    </row>
+    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A904" s="43"/>
+      <c r="B904" s="18"/>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A905" s="43"/>
+      <c r="B905" s="18"/>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A906" s="43"/>
+      <c r="B906" s="18"/>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A907" s="43"/>
+      <c r="B907" s="18"/>
+    </row>
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A908" s="43"/>
+      <c r="B908" s="18"/>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A909" s="43"/>
+      <c r="B909" s="18"/>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A910" s="43"/>
+      <c r="B910" s="18"/>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A911" s="43"/>
+      <c r="B911" s="18"/>
+    </row>
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A912" s="43"/>
+      <c r="B912" s="18"/>
+    </row>
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A913" s="43"/>
+      <c r="B913" s="18"/>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A914" s="43"/>
+      <c r="B914" s="18"/>
+    </row>
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A915" s="43"/>
+      <c r="B915" s="18"/>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A916" s="43"/>
+      <c r="B916" s="18"/>
+    </row>
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A917" s="43"/>
+      <c r="B917" s="18"/>
+    </row>
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A918" s="43"/>
+      <c r="B918" s="18"/>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A919" s="43"/>
+      <c r="B919" s="18"/>
+    </row>
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A920" s="43"/>
+      <c r="B920" s="18"/>
+    </row>
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A921" s="43"/>
+      <c r="B921" s="18"/>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A922" s="43"/>
+      <c r="B922" s="18"/>
+    </row>
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A923" s="43"/>
+      <c r="B923" s="18"/>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A924" s="43"/>
+      <c r="B924" s="18"/>
+    </row>
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A925" s="43"/>
+      <c r="B925" s="18"/>
+    </row>
+    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A926" s="43"/>
+      <c r="B926" s="18"/>
+    </row>
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A927" s="43"/>
+      <c r="B927" s="18"/>
+    </row>
+    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A928" s="43"/>
+      <c r="B928" s="18"/>
+    </row>
+    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A929" s="43"/>
+      <c r="B929" s="18"/>
+    </row>
+    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A930" s="43"/>
+      <c r="B930" s="18"/>
+    </row>
+    <row r="931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A931" s="43"/>
+      <c r="B931" s="18"/>
+    </row>
+    <row r="932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A932" s="43"/>
+      <c r="B932" s="18"/>
+    </row>
+    <row r="933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A933" s="43"/>
+      <c r="B933" s="18"/>
+    </row>
+    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A934" s="43"/>
+      <c r="B934" s="18"/>
+    </row>
+    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A935" s="43"/>
+      <c r="B935" s="18"/>
+    </row>
+    <row r="936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A936" s="43"/>
+      <c r="B936" s="18"/>
+    </row>
+    <row r="937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A937" s="43"/>
+      <c r="B937" s="18"/>
+    </row>
+    <row r="938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A938" s="43"/>
+      <c r="B938" s="18"/>
+    </row>
+    <row r="939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A939" s="43"/>
+      <c r="B939" s="18"/>
+    </row>
+    <row r="940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A940" s="43"/>
+      <c r="B940" s="18"/>
+    </row>
+    <row r="941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A941" s="43"/>
+      <c r="B941" s="18"/>
+    </row>
+    <row r="942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A942" s="43"/>
+      <c r="B942" s="18"/>
+    </row>
+    <row r="943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A943" s="43"/>
+      <c r="B943" s="18"/>
+    </row>
+    <row r="944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A944" s="43"/>
+      <c r="B944" s="18"/>
+    </row>
+    <row r="945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A945" s="43"/>
+      <c r="B945" s="18"/>
+    </row>
+    <row r="946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A946" s="43"/>
+      <c r="B946" s="18"/>
+    </row>
+    <row r="947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A947" s="43"/>
+      <c r="B947" s="18"/>
+    </row>
+    <row r="948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A948" s="43"/>
+      <c r="B948" s="18"/>
+    </row>
+    <row r="949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A949" s="43"/>
+      <c r="B949" s="18"/>
+    </row>
+    <row r="950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A950" s="43"/>
+      <c r="B950" s="18"/>
+    </row>
+    <row r="951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A951" s="43"/>
+      <c r="B951" s="18"/>
+    </row>
+    <row r="952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A952" s="43"/>
+      <c r="B952" s="18"/>
+    </row>
+    <row r="953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A953" s="43"/>
+      <c r="B953" s="18"/>
+    </row>
+    <row r="954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A954" s="43"/>
+      <c r="B954" s="24"/>
+    </row>
+    <row r="955" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A955" s="45"/>
+      <c r="B955" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
     <mergeCell ref="A316:A774"/>
-    <mergeCell ref="A778:A878"/>
+    <mergeCell ref="A778:A955"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizei o mq003 e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B660E-D204-4FF8-9FCF-DBE6AB1D13C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A61AD84-4A94-42BD-A5CA-46B75F1B19EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="452">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -25122,12 +25122,2170 @@
       <t xml:space="preserve"> ***</t>
     </r>
   </si>
+  <si>
+    <t>Aula 04 e 05 – Seguindo a orientação do dispositivo</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/style.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"all"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/retrato.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"screen and (orientation: portrait)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stylesheet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>href</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"estilos/paisagem.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"screen and (orientation: landscape)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Esse é o primeiro e o melhor exemplo de declaração de media type, é declarado no HTML cada declaração com o seu arquivo css separado</t>
+  </si>
+  <si>
+    <t>/* Aparelho deitado (landscape) */</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/cev-landscape.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>/* Aparelho em pé (portrait) */</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/cev-portrait.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>/* Configurações Gerais */</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#233eff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>contain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-repeat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>no-repeat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>text-shadow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#15267a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>paisagem.css</t>
+  </si>
+  <si>
+    <t>retrato.css</t>
+  </si>
+  <si>
+    <t>Esse é o segundo exemplo de declaração de media type, que também é bom, mas pode ser fácil de se confundir pois as medias ficam todas dentro do mesmo arquivo css. (somente css pq)</t>
+  </si>
+  <si>
+    <t>/*Declarações gerais*/</t>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>margin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>padding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>font-family</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Arial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Helvetica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sans-serif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#233eff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>contain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-repeat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>no-repeat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>white</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>text-shadow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#15267a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>padding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>/*Declarações retrato*/</t>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>orientation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>portrait</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/cev-portrait.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>/*Declarações paisagem*/</t>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>orientation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>landscape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/cev-landscape.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25362,8 +27520,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -25397,6 +27562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -25529,7 +27700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -25645,6 +27816,18 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -26053,10 +28236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
-  <dimension ref="A2:C955"/>
+  <dimension ref="A2:C1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A877" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B882" sqref="B882"/>
+    <sheetView tabSelected="1" topLeftCell="A1006" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1018" sqref="B1018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31004,244 +33187,786 @@
         <v>409</v>
       </c>
     </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A898" s="43"/>
       <c r="B898" s="18"/>
     </row>
-    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A899" s="43"/>
-      <c r="B899" s="18"/>
-    </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B899" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A900" s="43"/>
-      <c r="B900" s="18"/>
+      <c r="B900" s="41" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A901" s="43"/>
-      <c r="B901" s="18"/>
+      <c r="B901" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A902" s="43"/>
-      <c r="B902" s="18"/>
+      <c r="B902" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A903" s="43"/>
-      <c r="B903" s="18"/>
+      <c r="B903" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A904" s="43"/>
-      <c r="B904" s="18"/>
+      <c r="B904" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A905" s="43"/>
-      <c r="B905" s="18"/>
+      <c r="B905" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A906" s="43"/>
-      <c r="B906" s="18"/>
+      <c r="B906" s="3" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A907" s="43"/>
-      <c r="B907" s="18"/>
+      <c r="B907" s="3" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A908" s="43"/>
-      <c r="B908" s="18"/>
+      <c r="B908" s="3" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A909" s="43"/>
-      <c r="B909" s="18"/>
+      <c r="B909" s="3" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A910" s="43"/>
-      <c r="B910" s="18"/>
+      <c r="B910" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A911" s="43"/>
-      <c r="B911" s="18"/>
+      <c r="B911" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A912" s="43"/>
-      <c r="B912" s="18"/>
+      <c r="B912" s="3" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A913" s="43"/>
-      <c r="B913" s="18"/>
-    </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B913" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A914" s="43"/>
-      <c r="B914" s="18"/>
-    </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B914" s="47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A915" s="43"/>
-      <c r="B915" s="18"/>
+      <c r="B915" s="46" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A916" s="43"/>
-      <c r="B916" s="18"/>
+      <c r="B916" s="48" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A917" s="43"/>
-      <c r="B917" s="18"/>
+      <c r="B917" s="7"/>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A918" s="43"/>
-      <c r="B918" s="18"/>
+      <c r="B918" s="49" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A919" s="43"/>
-      <c r="B919" s="18"/>
+      <c r="B919" s="7"/>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A920" s="43"/>
-      <c r="B920" s="18"/>
+      <c r="B920" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A921" s="43"/>
-      <c r="B921" s="18"/>
+      <c r="B921" s="3" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A922" s="43"/>
-      <c r="B922" s="18"/>
+      <c r="B922" s="3" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A923" s="43"/>
-      <c r="B923" s="18"/>
-    </row>
-    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B923" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A924" s="43"/>
       <c r="B924" s="18"/>
     </row>
-    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A925" s="43"/>
-      <c r="B925" s="18"/>
+      <c r="B925" s="46" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A926" s="43"/>
-      <c r="B926" s="18"/>
+      <c r="B926" s="48" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A927" s="43"/>
-      <c r="B927" s="18"/>
+      <c r="B927" s="7"/>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A928" s="43"/>
-      <c r="B928" s="18"/>
+      <c r="B928" s="49" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A929" s="43"/>
-      <c r="B929" s="18"/>
+      <c r="B929" s="7"/>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A930" s="43"/>
-      <c r="B930" s="18"/>
+      <c r="B930" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A931" s="43"/>
-      <c r="B931" s="18"/>
+      <c r="B931" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A932" s="43"/>
-      <c r="B932" s="18"/>
+      <c r="B932" s="3" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A933" s="43"/>
-      <c r="B933" s="18"/>
-    </row>
-    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B933" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A934" s="43"/>
-      <c r="B934" s="18"/>
-    </row>
-    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B934" s="47"/>
+    </row>
+    <row r="935" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A935" s="43"/>
-      <c r="B935" s="18"/>
+      <c r="B935" s="46" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A936" s="43"/>
-      <c r="B936" s="18"/>
+      <c r="B936" s="48" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A937" s="43"/>
-      <c r="B937" s="18"/>
+      <c r="B937" s="7"/>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A938" s="43"/>
-      <c r="B938" s="18"/>
+      <c r="B938" s="49" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A939" s="43"/>
-      <c r="B939" s="18"/>
+      <c r="B939" s="7"/>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A940" s="43"/>
-      <c r="B940" s="18"/>
+      <c r="B940" s="14" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A941" s="43"/>
-      <c r="B941" s="18"/>
+      <c r="B941" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A942" s="43"/>
-      <c r="B942" s="18"/>
+      <c r="B942" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A943" s="43"/>
-      <c r="B943" s="18"/>
+      <c r="B943" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A944" s="43"/>
-      <c r="B944" s="18"/>
+      <c r="B944" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A945" s="43"/>
-      <c r="B945" s="18"/>
+      <c r="B945" s="7"/>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A946" s="43"/>
-      <c r="B946" s="18"/>
+      <c r="B946" s="14" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A947" s="43"/>
-      <c r="B947" s="18"/>
+      <c r="B947" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A948" s="43"/>
-      <c r="B948" s="18"/>
+      <c r="B948" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A949" s="43"/>
-      <c r="B949" s="18"/>
+      <c r="B949" s="3" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A950" s="43"/>
-      <c r="B950" s="18"/>
+      <c r="B950" s="3" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A951" s="43"/>
-      <c r="B951" s="18"/>
+      <c r="B951" s="3" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A952" s="43"/>
-      <c r="B952" s="18"/>
+      <c r="B952" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A953" s="43"/>
-      <c r="B953" s="18"/>
+      <c r="B953" s="7"/>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A954" s="43"/>
-      <c r="B954" s="24"/>
-    </row>
-    <row r="955" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A955" s="45"/>
-      <c r="B955" s="40"/>
+      <c r="B954" s="14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A955" s="43"/>
+      <c r="B955" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A956" s="43"/>
+      <c r="B956" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A957" s="43"/>
+      <c r="B957" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A958" s="43"/>
+      <c r="B958" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A959" s="43"/>
+      <c r="B959" s="3"/>
+    </row>
+    <row r="960" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A960" s="43"/>
+      <c r="B960" s="41" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A961" s="43"/>
+      <c r="B961" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A962" s="43"/>
+      <c r="B962" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A963" s="43"/>
+      <c r="B963" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A964" s="43"/>
+      <c r="B964" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A965" s="43"/>
+      <c r="B965" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A966" s="43"/>
+      <c r="B966" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A967" s="43"/>
+      <c r="B967" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A968" s="43"/>
+      <c r="B968" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A969" s="43"/>
+      <c r="B969" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A970" s="43"/>
+      <c r="B970" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A971" s="43"/>
+      <c r="B971" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A972" s="43"/>
+      <c r="B972" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A973" s="43"/>
+      <c r="B973" s="46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A974" s="43"/>
+      <c r="B974" s="3"/>
+    </row>
+    <row r="975" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A975" s="43"/>
+      <c r="B975" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A976" s="43"/>
+      <c r="B976" s="7"/>
+    </row>
+    <row r="977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A977" s="43"/>
+      <c r="B977" s="49" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="978" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A978" s="43"/>
+      <c r="B978" s="7"/>
+    </row>
+    <row r="979" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A979" s="43"/>
+      <c r="B979" s="14" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A980" s="43"/>
+      <c r="B980" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="981" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A981" s="43"/>
+      <c r="B981" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A982" s="43"/>
+      <c r="B982" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A983" s="43"/>
+      <c r="B983" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="984" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A984" s="43"/>
+      <c r="B984" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A985" s="43"/>
+      <c r="B985" s="7"/>
+    </row>
+    <row r="986" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A986" s="43"/>
+      <c r="B986" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="987" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A987" s="43"/>
+      <c r="B987" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="988" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A988" s="43"/>
+      <c r="B988" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="989" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A989" s="43"/>
+      <c r="B989" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A990" s="43"/>
+      <c r="B990" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="991" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A991" s="43"/>
+      <c r="B991" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="992" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A992" s="43"/>
+      <c r="B992" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="993" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A993" s="43"/>
+      <c r="B993" s="7"/>
+    </row>
+    <row r="994" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A994" s="43"/>
+      <c r="B994" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="995" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A995" s="43"/>
+      <c r="B995" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="996" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A996" s="43"/>
+      <c r="B996" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="997" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A997" s="43"/>
+      <c r="B997" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="998" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A998" s="43"/>
+      <c r="B998" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="999" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A999" s="43"/>
+      <c r="B999" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1000" s="43"/>
+      <c r="B1000" s="7"/>
+    </row>
+    <row r="1001" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1001" s="43"/>
+      <c r="B1001" s="49" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1002" s="43"/>
+      <c r="B1002" s="7"/>
+    </row>
+    <row r="1003" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1003" s="43"/>
+      <c r="B1003" s="14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1004" s="43"/>
+      <c r="B1004" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1005" s="43"/>
+      <c r="B1005" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1006" s="43"/>
+      <c r="B1006" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1007" s="43"/>
+      <c r="B1007" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1008" s="43"/>
+      <c r="B1008" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1009" s="43"/>
+      <c r="B1009" s="7"/>
+    </row>
+    <row r="1010" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1010" s="43"/>
+      <c r="B1010" s="49" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1011" s="43"/>
+      <c r="B1011" s="7"/>
+    </row>
+    <row r="1012" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1012" s="43"/>
+      <c r="B1012" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1013" s="43"/>
+      <c r="B1013" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1014" s="43"/>
+      <c r="B1014" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1015" s="43"/>
+      <c r="B1015" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1016" s="43"/>
+      <c r="B1016" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1017" s="43"/>
+      <c r="B1017" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1018" s="43"/>
+      <c r="B1018" s="47"/>
+    </row>
+    <row r="1019" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1019" s="43"/>
+      <c r="B1019" s="18"/>
+    </row>
+    <row r="1020" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1020" s="43"/>
+      <c r="B1020" s="18"/>
+    </row>
+    <row r="1021" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1021" s="43"/>
+      <c r="B1021" s="18"/>
+    </row>
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1022" s="43"/>
+      <c r="B1022" s="18"/>
+    </row>
+    <row r="1023" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1023" s="43"/>
+      <c r="B1023" s="18"/>
+    </row>
+    <row r="1024" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1024" s="43"/>
+      <c r="B1024" s="18"/>
+    </row>
+    <row r="1025" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1025" s="43"/>
+      <c r="B1025" s="18"/>
+    </row>
+    <row r="1026" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1026" s="43"/>
+      <c r="B1026" s="18"/>
+    </row>
+    <row r="1027" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1027" s="43"/>
+      <c r="B1027" s="18"/>
+    </row>
+    <row r="1028" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1028" s="43"/>
+      <c r="B1028" s="18"/>
+    </row>
+    <row r="1029" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1029" s="43"/>
+      <c r="B1029" s="18"/>
+    </row>
+    <row r="1030" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1030" s="43"/>
+      <c r="B1030" s="18"/>
+    </row>
+    <row r="1031" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1031" s="43"/>
+      <c r="B1031" s="18"/>
+    </row>
+    <row r="1032" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1032" s="43"/>
+      <c r="B1032" s="18"/>
+    </row>
+    <row r="1033" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1033" s="43"/>
+      <c r="B1033" s="18"/>
+    </row>
+    <row r="1034" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1034" s="43"/>
+      <c r="B1034" s="18"/>
+    </row>
+    <row r="1035" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1035" s="43"/>
+      <c r="B1035" s="18"/>
+    </row>
+    <row r="1036" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1036" s="43"/>
+      <c r="B1036" s="18"/>
+    </row>
+    <row r="1037" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1037" s="43"/>
+      <c r="B1037" s="18"/>
+    </row>
+    <row r="1038" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1038" s="43"/>
+      <c r="B1038" s="18"/>
+    </row>
+    <row r="1039" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1039" s="43"/>
+      <c r="B1039" s="18"/>
+    </row>
+    <row r="1040" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1040" s="43"/>
+      <c r="B1040" s="24"/>
+    </row>
+    <row r="1041" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1041" s="45"/>
+      <c r="B1041" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:A105"/>
     <mergeCell ref="A109:A312"/>
     <mergeCell ref="A316:A774"/>
-    <mergeCell ref="A778:A955"/>
+    <mergeCell ref="A778:A1041"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o media-query.css e planilha
</commit_message>
<xml_diff>
--- a/detalheshtmlecss.xlsx
+++ b/detalheshtmlecss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\html-e-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8343BF5-749A-4197-8C86-3D305937C121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3300A8C-0E78-4548-A897-AD0A112F6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3F6F84B5-039F-470A-A930-073CB1DDF646}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="506">
   <si>
     <t>https://www.youtube.com/watch?v=XTnr1DpHfKo</t>
   </si>
@@ -29295,6 +29295,1976 @@
   </si>
   <si>
     <t>Nessas img display none para ocultar as img, deixa display block para mostrar.</t>
+  </si>
+  <si>
+    <t>/* Todas as demais mídias */</t>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/*IMPRESSÃO*/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>font-family</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Courier New'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Courier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>monospace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/back-print.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">); </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/*NÃO PRECISA - NÃO IMPRIME..*/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>95</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>vw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>border</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>solid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>black</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>text-align</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>::</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>after</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Essa impressão foi feita através do site thiagocamponez.github.io'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>text-decoration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>overline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#phone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#tablet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>block</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#pc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#tv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>min-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>768</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>992</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/*TABLET*/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/back-tablet.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#tablet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>block</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>min-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>992</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) {   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/*DESKTOP*/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/back-pc.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#pc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>block</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;} </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>@media</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>min-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/* GRANDES TELAS */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>background-image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>../imagens/back-tv.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#tv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>block</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -29716,7 +31686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -29844,6 +31814,15 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -30254,8 +32233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DC79C-1361-4156-AA81-8DBF1E06B994}">
   <dimension ref="A2:C1187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1072" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1098" sqref="B1098"/>
+    <sheetView tabSelected="1" topLeftCell="A1132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1099" sqref="B1099"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36333,13 +38312,15 @@
         <v>479</v>
       </c>
     </row>
-    <row r="1098" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1098" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1098" s="47"/>
       <c r="B1098" s="18"/>
     </row>
-    <row r="1099" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1099" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1099" s="47"/>
-      <c r="B1099" s="18"/>
+      <c r="B1099" s="42" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1100" s="47"/>
@@ -36347,271 +38328,383 @@
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1101" s="47"/>
-      <c r="B1101" s="18"/>
+      <c r="B1101" s="50" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1102" s="47"/>
-      <c r="B1102" s="18"/>
+      <c r="B1102" s="51"/>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1103" s="47"/>
-      <c r="B1103" s="18"/>
+      <c r="B1103" s="52" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1104" s="47"/>
-      <c r="B1104" s="18"/>
+      <c r="B1104" s="51"/>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1105" s="47"/>
-      <c r="B1105" s="18"/>
+      <c r="B1105" s="50" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1106" s="47"/>
-      <c r="B1106" s="18"/>
+      <c r="B1106" s="51"/>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1107" s="47"/>
-      <c r="B1107" s="18"/>
+      <c r="B1107" s="29" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1108" s="47"/>
-      <c r="B1108" s="18"/>
+      <c r="B1108" s="29" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1109" s="47"/>
-      <c r="B1109" s="18"/>
+      <c r="B1109" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1110" s="47"/>
-      <c r="B1110" s="18"/>
+      <c r="B1110" s="29" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1111" s="47"/>
-      <c r="B1111" s="18"/>
+      <c r="B1111" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1112" s="47"/>
-      <c r="B1112" s="18"/>
+      <c r="B1112" s="29" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1113" s="47"/>
-      <c r="B1113" s="18"/>
+      <c r="B1113" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1114" s="47"/>
-      <c r="B1114" s="18"/>
+      <c r="B1114" s="29" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1115" s="47"/>
-      <c r="B1115" s="18"/>
+      <c r="B1115" s="29" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1116" s="47"/>
-      <c r="B1116" s="18"/>
+      <c r="B1116" s="29" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1117" s="47"/>
-      <c r="B1117" s="18"/>
+      <c r="B1117" s="29" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1118" s="47"/>
-      <c r="B1118" s="18"/>
+      <c r="B1118" s="29" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1119" s="47"/>
-      <c r="B1119" s="18"/>
+      <c r="B1119" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1120" s="47"/>
-      <c r="B1120" s="18"/>
+      <c r="B1120" s="51"/>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1121" s="47"/>
-      <c r="B1121" s="18"/>
+      <c r="B1121" s="29" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1122" s="47"/>
-      <c r="B1122" s="18"/>
+      <c r="B1122" s="29" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1123" s="47"/>
-      <c r="B1123" s="18"/>
+      <c r="B1123" s="29" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1124" s="47"/>
-      <c r="B1124" s="18"/>
+      <c r="B1124" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1125" s="47"/>
-      <c r="B1125" s="18"/>
+      <c r="B1125" s="51"/>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1126" s="47"/>
-      <c r="B1126" s="18"/>
+      <c r="B1126" s="29" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1127" s="47"/>
-      <c r="B1127" s="18"/>
+      <c r="B1127" s="29" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1128" s="47"/>
-      <c r="B1128" s="18"/>
+      <c r="B1128" s="29" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1129" s="47"/>
-      <c r="B1129" s="18"/>
+      <c r="B1129" s="29" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1130" s="47"/>
-      <c r="B1130" s="18"/>
+      <c r="B1130" s="29" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1131" s="47"/>
-      <c r="B1131" s="18"/>
+      <c r="B1131" s="29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1132" s="47"/>
-      <c r="B1132" s="18"/>
+      <c r="B1132" s="51"/>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1133" s="47"/>
-      <c r="B1133" s="18"/>
+      <c r="B1133" s="50" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1134" s="47"/>
-      <c r="B1134" s="18"/>
+      <c r="B1134" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1135" s="47"/>
-      <c r="B1135" s="18"/>
+      <c r="B1135" s="29" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1136" s="47"/>
-      <c r="B1136" s="18"/>
+      <c r="B1136" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1137" s="47"/>
-      <c r="B1137" s="18"/>
+      <c r="B1137" s="51"/>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1138" s="47"/>
-      <c r="B1138" s="18"/>
+      <c r="B1138" s="29" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1139" s="47"/>
-      <c r="B1139" s="18"/>
+      <c r="B1139" s="29" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1140" s="47"/>
-      <c r="B1140" s="18"/>
+      <c r="B1140" s="29" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1141" s="47"/>
-      <c r="B1141" s="18"/>
+      <c r="B1141" s="29" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1142" s="47"/>
-      <c r="B1142" s="18"/>
+      <c r="B1142" s="29" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1143" s="47"/>
-      <c r="B1143" s="18"/>
+      <c r="B1143" s="29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1144" s="47"/>
-      <c r="B1144" s="18"/>
+      <c r="B1144" s="51"/>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1145" s="47"/>
-      <c r="B1145" s="18"/>
+      <c r="B1145" s="50" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1146" s="47"/>
-      <c r="B1146" s="18"/>
+      <c r="B1146" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1147" s="47"/>
-      <c r="B1147" s="18"/>
+      <c r="B1147" s="29" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1148" s="47"/>
-      <c r="B1148" s="18"/>
+      <c r="B1148" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1149" s="47"/>
-      <c r="B1149" s="18"/>
+      <c r="B1149" s="51"/>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1150" s="47"/>
-      <c r="B1150" s="18"/>
+      <c r="B1150" s="29" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1151" s="47"/>
-      <c r="B1151" s="18"/>
+      <c r="B1151" s="29" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1152" s="47"/>
-      <c r="B1152" s="18"/>
+      <c r="B1152" s="29" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1153" s="47"/>
-      <c r="B1153" s="18"/>
+      <c r="B1153" s="29" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1154" s="47"/>
-      <c r="B1154" s="18"/>
+      <c r="B1154" s="29" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1155" s="47"/>
-      <c r="B1155" s="18"/>
+      <c r="B1155" s="29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1156" s="47"/>
-      <c r="B1156" s="18"/>
+      <c r="B1156" s="51"/>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1157" s="47"/>
-      <c r="B1157" s="18"/>
+      <c r="B1157" s="50" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1158" s="47"/>
-      <c r="B1158" s="18"/>
+      <c r="B1158" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1159" s="47"/>
-      <c r="B1159" s="18"/>
+      <c r="B1159" s="29" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1160" s="47"/>
-      <c r="B1160" s="18"/>
+      <c r="B1160" s="29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="1161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1161" s="47"/>
-      <c r="B1161" s="18"/>
+      <c r="B1161" s="51"/>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1162" s="47"/>
-      <c r="B1162" s="18"/>
+      <c r="B1162" s="29" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1163" s="47"/>
-      <c r="B1163" s="18"/>
+      <c r="B1163" s="29" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1164" s="47"/>
-      <c r="B1164" s="18"/>
+      <c r="B1164" s="29" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1165" s="47"/>
-      <c r="B1165" s="18"/>
+      <c r="B1165" s="29" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1166" s="47"/>
-      <c r="B1166" s="18"/>
+      <c r="B1166" s="29" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1167" s="47"/>
-      <c r="B1167" s="18"/>
+      <c r="B1167" s="29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="1168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1168" s="47"/>

</xml_diff>